<commit_message>
feat: update severity in json file
</commit_message>
<xml_diff>
--- a/report/coba.xlsx
+++ b/report/coba.xlsx
@@ -1181,7 +1181,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1208,13 +1208,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1296,13 +1289,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1940,7 +1933,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -2030,7 +2023,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -2113,7 +2106,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B34" s="7" t="s">
@@ -2143,7 +2136,7 @@
       <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -2256,7 +2249,7 @@
       <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -2331,7 +2324,7 @@
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B49" s="7" t="s">
@@ -2384,7 +2377,7 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B53" s="7" t="s">
@@ -2399,7 +2392,7 @@
       <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>132</v>
       </c>
       <c r="B54" s="7" t="s">
@@ -2414,7 +2407,7 @@
       <c r="G54" s="7"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B55" s="7" t="s">
@@ -3103,7 +3096,7 @@
       <c r="G112" s="7"/>
     </row>
     <row r="113" spans="1:7">
-      <c r="A113" s="5" t="s">
+      <c r="A113" s="4" t="s">
         <v>217</v>
       </c>
       <c r="B113" s="7" t="s">
@@ -3156,7 +3149,7 @@
       <c r="G116" s="7"/>
     </row>
     <row r="117" spans="1:7">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="4" t="s">
         <v>224</v>
       </c>
       <c r="B117" s="7" t="s">
@@ -3988,7 +3981,7 @@
       <c r="G190" s="7"/>
     </row>
     <row r="191" spans="1:7">
-      <c r="A191" s="5" t="s">
+      <c r="A191" s="3" t="s">
         <v>244</v>
       </c>
       <c r="B191" s="7" t="s">
@@ -4003,7 +3996,7 @@
       <c r="G191" s="7"/>
     </row>
     <row r="192" spans="1:7">
-      <c r="A192" s="5" t="s">
+      <c r="A192" s="4" t="s">
         <v>247</v>
       </c>
       <c r="B192" s="7" t="s">
@@ -4018,7 +4011,7 @@
       <c r="G192" s="7"/>
     </row>
     <row r="193" spans="1:7">
-      <c r="A193" s="5" t="s">
+      <c r="A193" s="3" t="s">
         <v>250</v>
       </c>
       <c r="B193" s="7" t="s">
@@ -4033,7 +4026,7 @@
       <c r="G193" s="7"/>
     </row>
     <row r="194" spans="1:7">
-      <c r="A194" s="5" t="s">
+      <c r="A194" s="4" t="s">
         <v>253</v>
       </c>
       <c r="B194" s="7" t="s">
@@ -4063,7 +4056,7 @@
       <c r="G195" s="7"/>
     </row>
     <row r="196" spans="1:7">
-      <c r="A196" s="5" t="s">
+      <c r="A196" s="3" t="s">
         <v>259</v>
       </c>
       <c r="B196" s="7" t="s">
@@ -4078,7 +4071,7 @@
       <c r="G196" s="7"/>
     </row>
     <row r="197" spans="1:7">
-      <c r="A197" s="5" t="s">
+      <c r="A197" s="3" t="s">
         <v>262</v>
       </c>
       <c r="B197" s="7" t="s">
@@ -4093,7 +4086,7 @@
       <c r="G197" s="7"/>
     </row>
     <row r="198" spans="1:7">
-      <c r="A198" s="5" t="s">
+      <c r="A198" s="4" t="s">
         <v>265</v>
       </c>
       <c r="B198" s="7" t="s">
@@ -4108,7 +4101,7 @@
       <c r="G198" s="7"/>
     </row>
     <row r="199" spans="1:7">
-      <c r="A199" s="5" t="s">
+      <c r="A199" s="4" t="s">
         <v>267</v>
       </c>
       <c r="B199" s="7" t="s">
@@ -4123,7 +4116,7 @@
       <c r="G199" s="7"/>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="5" t="s">
+      <c r="A200" s="4" t="s">
         <v>270</v>
       </c>
       <c r="B200" s="7" t="s">
@@ -4138,7 +4131,7 @@
       <c r="G200" s="7"/>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="5" t="s">
+      <c r="A201" s="4" t="s">
         <v>273</v>
       </c>
       <c r="B201" s="7" t="s">
@@ -4168,7 +4161,7 @@
       <c r="G202" s="7"/>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="5" t="s">
+      <c r="A203" s="4" t="s">
         <v>279</v>
       </c>
       <c r="B203" s="7" t="s">
@@ -4183,7 +4176,7 @@
       <c r="G203" s="7"/>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="5" t="s">
+      <c r="A204" s="3" t="s">
         <v>282</v>
       </c>
       <c r="B204" s="7" t="s">
@@ -4198,7 +4191,7 @@
       <c r="G204" s="7"/>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="5" t="s">
+      <c r="A205" s="4" t="s">
         <v>285</v>
       </c>
       <c r="B205" s="7" t="s">
@@ -4387,7 +4380,7 @@
       </c>
     </row>
     <row r="219" spans="1:7">
-      <c r="A219" s="5" t="s">
+      <c r="A219" s="4" t="s">
         <v>311</v>
       </c>
       <c r="B219" s="7" t="s">
@@ -4507,7 +4500,7 @@
       <c r="G226" s="7"/>
     </row>
     <row r="227" spans="1:7">
-      <c r="A227" s="5" t="s">
+      <c r="A227" s="4" t="s">
         <v>335</v>
       </c>
       <c r="B227" s="7" t="s">
@@ -4522,7 +4515,7 @@
       <c r="G227" s="7"/>
     </row>
     <row r="228" spans="1:7">
-      <c r="A228" s="5" t="s">
+      <c r="A228" s="4" t="s">
         <v>338</v>
       </c>
       <c r="B228" s="7" t="s">
@@ -4560,7 +4553,7 @@
       </c>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="5" t="s">
+      <c r="A231" s="4" t="s">
         <v>342</v>
       </c>
       <c r="B231" s="7" t="s">
@@ -4793,7 +4786,7 @@
       </c>
     </row>
     <row r="247" spans="1:7">
-      <c r="A247" s="5" t="s">
+      <c r="A247" s="4" t="s">
         <v>384</v>
       </c>
       <c r="B247" s="7" t="s">

</xml_diff>

<commit_message>
feat: optimize mapper feature, check redundant url, files url
</commit_message>
<xml_diff>
--- a/report/coba.xlsx
+++ b/report/coba.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="357">
   <si>
     <t>OWASP: Testing Guide v4.2 Checklist</t>
   </si>
@@ -433,310 +433,220 @@
     <t>GET http://192.168.1.4:3000/api/Addresss</t>
   </si>
   <si>
+    <t>GET http://192.168.1.4:3000/api/Addresss/&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Cards</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Cards/&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Deliverys</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Feedbacks/</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Quantitys/</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/rest/admin/application-configuration</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/rest/basket/&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/rest/captcha/</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/rest/products/search?q=</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/rest/user/whoami</t>
+  </si>
+  <si>
+    <t>WSTG-ATHZ-04</t>
+  </si>
+  <si>
+    <t>Testing for Insecure Direct Object References</t>
+  </si>
+  <si>
+    <t>- Identify points where object references may occur.- Assess the access control measures and if they're vulnerable to IDOR.</t>
+  </si>
+  <si>
+    <t>WSTG-ATHZ-05</t>
+  </si>
+  <si>
+    <t>Testing for OAuth Weaknesses</t>
+  </si>
+  <si>
+    <t>- Determine if OAuth2 implementation is vulnerable or using a deprecated or custom implementation.</t>
+  </si>
+  <si>
+    <t>Session Management Testing</t>
+  </si>
+  <si>
+    <t>WSTG-SESS-01</t>
+  </si>
+  <si>
+    <t>Testing for Session Management Schema</t>
+  </si>
+  <si>
+    <t>- Gather session tokens, for the same user and for different users where possible.- Analyze and ensure that enough randomness exists to stop session forging attacks.- Modify cookies that are not signed and contain information that can be manipulated.</t>
+  </si>
+  <si>
+    <t>WSTG-SESS-02</t>
+  </si>
+  <si>
+    <t>Testing for Cookies Attributes</t>
+  </si>
+  <si>
+    <t>- Ensure that the proper security configuration is set for cookies.</t>
+  </si>
+  <si>
+    <t>WSTG-SESS-03</t>
+  </si>
+  <si>
+    <t>Testing for Session Fixation</t>
+  </si>
+  <si>
+    <t>- Analyze the authentication mechanism and its flow.- Force cookies and assess the impact.</t>
+  </si>
+  <si>
+    <t>WSTG-SESS-04</t>
+  </si>
+  <si>
+    <t>Testing for Exposed Session Variables</t>
+  </si>
+  <si>
+    <t>- Ensure that proper encryption is implemented.- Review the caching configuration.- Assess the channel and methods' security.</t>
+  </si>
+  <si>
+    <t>WSTG-SESS-05</t>
+  </si>
+  <si>
+    <t>Testing for Cross Site Request Forgery</t>
+  </si>
+  <si>
+    <t>- Determine whether it is possible to initiate requests on a user's behalf that are not initiated by the user.</t>
+  </si>
+  <si>
+    <t>WSTG-SESS-06</t>
+  </si>
+  <si>
+    <t>Testing for Logout Functionality</t>
+  </si>
+  <si>
+    <t>- Assess the logout UI.- Analyze the session timeout and if the session is properly killed after logout.</t>
+  </si>
+  <si>
+    <t>WSTG-SESS-07</t>
+  </si>
+  <si>
+    <t>Testing Session Timeout</t>
+  </si>
+  <si>
+    <t>- Validate that a hard session timeout exists.</t>
+  </si>
+  <si>
+    <t>WSTG-SESS-08</t>
+  </si>
+  <si>
+    <t>Testing for Session Puzzling</t>
+  </si>
+  <si>
+    <t>- Identify all session variables.- Break the logical flow of session generation.</t>
+  </si>
+  <si>
+    <t>WSTG-SESS-09</t>
+  </si>
+  <si>
+    <t>Testing for Session Hijacking</t>
+  </si>
+  <si>
+    <t>- Identify vulnerable session cookies.- Hijack vulnerable cookies and assess the risk level.</t>
+  </si>
+  <si>
+    <t>WSTG-SESS-10</t>
+  </si>
+  <si>
+    <t>Testing JSON Web Tokens</t>
+  </si>
+  <si>
+    <t>- Determine whether the JWTs expose sensitive information.- Determine whether the JWTs can be tampered with or modified.</t>
+  </si>
+  <si>
+    <t>Input Validation Testing</t>
+  </si>
+  <si>
+    <t>WSTG-INPV-01</t>
+  </si>
+  <si>
+    <t>Testing for Reflected Cross Site Scripting</t>
+  </si>
+  <si>
+    <t>- Identify variables that are reflected in responses.- Assess the input they accept and the encoding that gets applied on return (if any).</t>
+  </si>
+  <si>
+    <t>WSTG-INPV-02</t>
+  </si>
+  <si>
+    <t>Testing for Stored Cross Site Scripting</t>
+  </si>
+  <si>
+    <t>- Identify stored input that is reflected on the client-side.- Assess the input they accept and the encoding that gets applied on return (if any).</t>
+  </si>
+  <si>
+    <t>WSTG-INPV-03</t>
+  </si>
+  <si>
+    <t>Testing for HTTP Verb Tampering</t>
+  </si>
+  <si>
+    <t>WSTG-INPV-04</t>
+  </si>
+  <si>
+    <t>Testing for HTTP Parameter Pollution</t>
+  </si>
+  <si>
+    <t>- Identify the backend and the parsing method used.- Assess injection points and try bypassing input filters using HPP.</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/</t>
+  </si>
+  <si>
     <t>POST http://192.168.1.4:3000/api/Addresss/</t>
   </si>
   <si>
-    <t>GET http://192.168.1.4:3000/api/Addresss/7</t>
-  </si>
-  <si>
     <t>POST http://192.168.1.4:3000/api/BasketItems/</t>
   </si>
   <si>
-    <t>GET http://192.168.1.4:3000/api/Cards</t>
-  </si>
-  <si>
     <t>POST http://192.168.1.4:3000/api/Cards/</t>
   </si>
   <si>
-    <t>GET http://192.168.1.4:3000/api/Cards/7</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Challenges/?name=Score%20Board</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Deliverys</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Deliverys/1</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Feedbacks/</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Products/1?d=Mon%20May%2001%202023</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Quantitys/</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/assets/i18n/en.json</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/assets/public/images/uploads/%F0%9F%98%BC-</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/admin/application-configuration</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/admin/application-version</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/basket/6</t>
-  </si>
-  <si>
-    <t>POST http://192.168.1.4:3000/rest/basket/6/checkout</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/captcha/</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/languages</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/products/search?q=</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/track-order/1aed-d26768198c07c8e6</t>
+    <t>GET http://192.168.1.4:3000/api/Challenges/?name=&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Deliverys/&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Products/?d=&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>POST http://192.168.1.4:3000/api/SecurityAnswers/</t>
+  </si>
+  <si>
+    <t>POST http://192.168.1.4:3000/api/Users/</t>
   </si>
   <si>
     <t>POST http://192.168.1.4:3000/rest/user/login</t>
   </si>
   <si>
-    <t>GET http://192.168.1.4:3000/rest/user/whoami</t>
-  </si>
-  <si>
     <t>GET http://192.168.1.4:3000/rest/wallet/balance</t>
   </si>
   <si>
-    <t>POST http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMvWFC&amp;sid=p28FbR6RsbcZU0fRAAAK</t>
-  </si>
-  <si>
-    <t>POST http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMvQAt&amp;sid=p28FbR6RsbcZU0fRAAAK</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMv-9E.0&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMviTA&amp;sid=p28FbR6RsbcZU0fRAAAK</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMvoaU.0&amp;sid=p28FbR6RsbcZU0fRAAAK</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMvu1W</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMvu3K.0&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMvu3j&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMw4Ga&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMwANj&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMwGU-&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMwMcF&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMwSjE&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMwYqU&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMwexm.0&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMwl2u&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMwr9y&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMwxG-&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMx1OC&amp;sid=0MSLG-Rna4r48aXdAAAM</t>
-  </si>
-  <si>
-    <t>WSTG-ATHZ-04</t>
-  </si>
-  <si>
-    <t>Testing for Insecure Direct Object References</t>
-  </si>
-  <si>
-    <t>- Identify points where object references may occur.- Assess the access control measures and if they're vulnerable to IDOR.</t>
-  </si>
-  <si>
-    <t>WSTG-ATHZ-05</t>
-  </si>
-  <si>
-    <t>Testing for OAuth Weaknesses</t>
-  </si>
-  <si>
-    <t>- Determine if OAuth2 implementation is vulnerable or using a deprecated or custom implementation.</t>
-  </si>
-  <si>
-    <t>Session Management Testing</t>
-  </si>
-  <si>
-    <t>WSTG-SESS-01</t>
-  </si>
-  <si>
-    <t>Testing for Session Management Schema</t>
-  </si>
-  <si>
-    <t>- Gather session tokens, for the same user and for different users where possible.- Analyze and ensure that enough randomness exists to stop session forging attacks.- Modify cookies that are not signed and contain information that can be manipulated.</t>
-  </si>
-  <si>
-    <t>WSTG-SESS-02</t>
-  </si>
-  <si>
-    <t>Testing for Cookies Attributes</t>
-  </si>
-  <si>
-    <t>- Ensure that the proper security configuration is set for cookies.</t>
-  </si>
-  <si>
-    <t>WSTG-SESS-03</t>
-  </si>
-  <si>
-    <t>Testing for Session Fixation</t>
-  </si>
-  <si>
-    <t>- Analyze the authentication mechanism and its flow.- Force cookies and assess the impact.</t>
-  </si>
-  <si>
-    <t>WSTG-SESS-04</t>
-  </si>
-  <si>
-    <t>Testing for Exposed Session Variables</t>
-  </si>
-  <si>
-    <t>- Ensure that proper encryption is implemented.- Review the caching configuration.- Assess the channel and methods' security.</t>
-  </si>
-  <si>
-    <t>WSTG-SESS-05</t>
-  </si>
-  <si>
-    <t>Testing for Cross Site Request Forgery</t>
-  </si>
-  <si>
-    <t>- Determine whether it is possible to initiate requests on a user's behalf that are not initiated by the user.</t>
-  </si>
-  <si>
-    <t>WSTG-SESS-06</t>
-  </si>
-  <si>
-    <t>Testing for Logout Functionality</t>
-  </si>
-  <si>
-    <t>- Assess the logout UI.- Analyze the session timeout and if the session is properly killed after logout.</t>
-  </si>
-  <si>
-    <t>WSTG-SESS-07</t>
-  </si>
-  <si>
-    <t>Testing Session Timeout</t>
-  </si>
-  <si>
-    <t>- Validate that a hard session timeout exists.</t>
-  </si>
-  <si>
-    <t>WSTG-SESS-08</t>
-  </si>
-  <si>
-    <t>Testing for Session Puzzling</t>
-  </si>
-  <si>
-    <t>- Identify all session variables.- Break the logical flow of session generation.</t>
-  </si>
-  <si>
-    <t>WSTG-SESS-09</t>
-  </si>
-  <si>
-    <t>Testing for Session Hijacking</t>
-  </si>
-  <si>
-    <t>- Identify vulnerable session cookies.- Hijack vulnerable cookies and assess the risk level.</t>
-  </si>
-  <si>
-    <t>WSTG-SESS-10</t>
-  </si>
-  <si>
-    <t>Testing JSON Web Tokens</t>
-  </si>
-  <si>
-    <t>- Determine whether the JWTs expose sensitive information.- Determine whether the JWTs can be tampered with or modified.</t>
-  </si>
-  <si>
-    <t>Input Validation Testing</t>
-  </si>
-  <si>
-    <t>WSTG-INPV-01</t>
-  </si>
-  <si>
-    <t>Testing for Reflected Cross Site Scripting</t>
-  </si>
-  <si>
-    <t>- Identify variables that are reflected in responses.- Assess the input they accept and the encoding that gets applied on return (if any).</t>
-  </si>
-  <si>
-    <t>WSTG-INPV-02</t>
-  </si>
-  <si>
-    <t>Testing for Stored Cross Site Scripting</t>
-  </si>
-  <si>
-    <t>- Identify stored input that is reflected on the client-side.- Assess the input they accept and the encoding that gets applied on return (if any).</t>
-  </si>
-  <si>
-    <t>WSTG-INPV-03</t>
-  </si>
-  <si>
-    <t>Testing for HTTP Verb Tampering</t>
-  </si>
-  <si>
-    <t>WSTG-INPV-04</t>
-  </si>
-  <si>
-    <t>Testing for HTTP Parameter Pollution</t>
-  </si>
-  <si>
-    <t>- Identify the backend and the parsing method used.- Assess injection points and try bypassing input filters using HPP.</t>
-  </si>
-  <si>
-    <t>POST http://192.168.1.4:3000/api/SecurityAnswers/</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/SecurityQuestions/</t>
-  </si>
-  <si>
-    <t>POST http://192.168.1.4:3000/api/Users/</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/favicon.ico</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMvQ7m</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMvQAt.0&amp;sid=p28FbR6RsbcZU0fRAAAK</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMvQBS&amp;sid=p28FbR6RsbcZU0fRAAAK</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMvWFC.0&amp;sid=p28FbR6RsbcZU0fRAAAK</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=4&amp;transport=polling&amp;t=OVMvcMD.0&amp;sid=p28FbR6RsbcZU0fRAAAK</t>
+    <t>GET http://192.168.1.4:3000/socket.io/?EIO=&lt;value&gt;&amp;transport=&lt;value&gt;&amp;t=&lt;value&gt;&amp;sid=&lt;value&gt;</t>
   </si>
   <si>
     <t>WSTG-INPV-05</t>
@@ -1649,7 +1559,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G247"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2423,13 +2333,13 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="4" t="s">
-        <v>183</v>
+        <v>150</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>138</v>
@@ -2560,415 +2470,482 @@
       <c r="G67" s="7"/>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="4"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7" t="s">
-        <v>150</v>
-      </c>
+      <c r="A68" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
     </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="4"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E69" s="7"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
-    </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="4"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
+      <c r="A70" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="4"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7" t="s">
-        <v>153</v>
-      </c>
+      <c r="A71" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D71" s="7"/>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="4"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7" t="s">
-        <v>154</v>
-      </c>
+      <c r="A72" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D72" s="7"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="4"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7" t="s">
-        <v>155</v>
-      </c>
+      <c r="A73" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D73" s="7"/>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="4"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7" t="s">
-        <v>156</v>
-      </c>
+      <c r="A74" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D74" s="7"/>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="4"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7" t="s">
-        <v>157</v>
-      </c>
+      <c r="A75" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D75" s="7"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="4"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7" t="s">
-        <v>158</v>
-      </c>
+      <c r="A76" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="4"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7" t="s">
-        <v>159</v>
-      </c>
+      <c r="A77" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D77" s="7"/>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="4"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7" t="s">
-        <v>160</v>
-      </c>
+      <c r="A78" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="4"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="A79" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D79" s="7"/>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="4"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7" t="s">
-        <v>162</v>
-      </c>
+      <c r="A80" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D80" s="7"/>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
     </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="4"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
-      <c r="D81" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E81" s="7"/>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7"/>
-    </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="4"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
+      <c r="A82" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="4"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="7" t="s">
-        <v>165</v>
-      </c>
+      <c r="A83" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D83" s="7"/>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="4"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="7" t="s">
-        <v>166</v>
-      </c>
+      <c r="A84" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D84" s="7"/>
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="4"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="7"/>
-      <c r="D85" s="7" t="s">
-        <v>167</v>
-      </c>
+      <c r="A85" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D85" s="7"/>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="4"/>
-      <c r="B86" s="7"/>
-      <c r="C86" s="7"/>
-      <c r="D86" s="7" t="s">
-        <v>168</v>
-      </c>
+      <c r="A86" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D86" s="7"/>
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="4"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
+      <c r="A87" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>213</v>
+      </c>
       <c r="D87" s="7" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
     </row>
     <row r="88" spans="1:7">
-      <c r="A88" s="4"/>
+      <c r="A88" s="3"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7" t="s">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="4"/>
+      <c r="A89" s="3"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="4"/>
+      <c r="A90" s="3"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="4"/>
+      <c r="A91" s="3"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
     </row>
     <row r="92" spans="1:7">
-      <c r="A92" s="4"/>
+      <c r="A92" s="3"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7" t="s">
-        <v>174</v>
+        <v>204</v>
       </c>
       <c r="E92" s="7"/>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
     </row>
     <row r="93" spans="1:7">
-      <c r="A93" s="4"/>
+      <c r="A93" s="3"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7" t="s">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
     </row>
     <row r="94" spans="1:7">
-      <c r="A94" s="4"/>
+      <c r="A94" s="3"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
     </row>
     <row r="95" spans="1:7">
-      <c r="A95" s="4"/>
+      <c r="A95" s="3"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
     </row>
     <row r="96" spans="1:7">
-      <c r="A96" s="4"/>
+      <c r="A96" s="3"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="4"/>
+      <c r="A97" s="3"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
     </row>
     <row r="98" spans="1:7">
-      <c r="A98" s="4"/>
+      <c r="A98" s="3"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
     </row>
     <row r="99" spans="1:7">
-      <c r="A99" s="4"/>
+      <c r="A99" s="3"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
     </row>
     <row r="100" spans="1:7">
-      <c r="A100" s="4"/>
+      <c r="A100" s="3"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
     <row r="101" spans="1:7">
-      <c r="A101" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B101" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D101" s="7"/>
+      <c r="A101" s="3"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7" t="s">
+        <v>209</v>
+      </c>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
       <c r="G101" s="7"/>
     </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="3"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
+    </row>
     <row r="103" spans="1:7">
-      <c r="A103" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F103" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G103" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A103" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="7"/>
     </row>
     <row r="104" spans="1:7">
-      <c r="A104" s="5" t="s">
-        <v>190</v>
+      <c r="A104" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>192</v>
+        <v>219</v>
       </c>
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
@@ -2976,14 +2953,14 @@
       <c r="G104" s="7"/>
     </row>
     <row r="105" spans="1:7">
-      <c r="A105" s="5" t="s">
-        <v>193</v>
+      <c r="A105" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
@@ -2991,14 +2968,14 @@
       <c r="G105" s="7"/>
     </row>
     <row r="106" spans="1:7">
-      <c r="A106" s="5" t="s">
-        <v>196</v>
+      <c r="A106" s="4" t="s">
+        <v>223</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>197</v>
+        <v>224</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
@@ -3007,13 +2984,13 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="5" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
@@ -3021,14 +2998,14 @@
       <c r="G107" s="7"/>
     </row>
     <row r="108" spans="1:7">
-      <c r="A108" s="5" t="s">
-        <v>202</v>
+      <c r="A108" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>203</v>
+        <v>230</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
@@ -3036,14 +3013,14 @@
       <c r="G108" s="7"/>
     </row>
     <row r="109" spans="1:7">
-      <c r="A109" s="5" t="s">
-        <v>205</v>
+      <c r="A109" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
@@ -3051,14 +3028,14 @@
       <c r="G109" s="7"/>
     </row>
     <row r="110" spans="1:7">
-      <c r="A110" s="5" t="s">
-        <v>208</v>
+      <c r="A110" s="4" t="s">
+        <v>235</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>210</v>
+        <v>39</v>
       </c>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
@@ -3066,14 +3043,14 @@
       <c r="G110" s="7"/>
     </row>
     <row r="111" spans="1:7">
-      <c r="A111" s="5" t="s">
-        <v>211</v>
+      <c r="A111" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
@@ -3081,14 +3058,14 @@
       <c r="G111" s="7"/>
     </row>
     <row r="112" spans="1:7">
-      <c r="A112" s="5" t="s">
-        <v>214</v>
+      <c r="A112" s="4" t="s">
+        <v>240</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>215</v>
+        <v>241</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
@@ -3097,51 +3074,58 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="4" t="s">
-        <v>217</v>
+        <v>243</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
       <c r="F113" s="7"/>
       <c r="G113" s="7"/>
     </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="D114" s="7"/>
+      <c r="E114" s="7"/>
+      <c r="F114" s="7"/>
+      <c r="G114" s="7"/>
+    </row>
     <row r="115" spans="1:7">
-      <c r="A115" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E115" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F115" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G115" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A115" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7"/>
     </row>
     <row r="116" spans="1:7">
-      <c r="A116" s="5" t="s">
-        <v>221</v>
+      <c r="A116" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>223</v>
+        <v>254</v>
       </c>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
@@ -3150,13 +3134,13 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117" s="4" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>226</v>
+        <v>257</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
@@ -3165,1655 +3149,613 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="5" t="s">
-        <v>227</v>
+        <v>258</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>228</v>
+        <v>259</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>39</v>
+        <v>260</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
       <c r="F118" s="7"/>
       <c r="G118" s="7"/>
     </row>
-    <row r="119" spans="1:7">
-      <c r="A119" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="D119" s="7"/>
-      <c r="E119" s="7"/>
-      <c r="F119" s="7"/>
-      <c r="G119" s="7"/>
-    </row>
     <row r="120" spans="1:7">
-      <c r="A120" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E120" s="7"/>
-      <c r="F120" s="7"/>
-      <c r="G120" s="7"/>
+      <c r="A120" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G120" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="121" spans="1:7">
-      <c r="A121" s="3"/>
-      <c r="B121" s="7"/>
-      <c r="C121" s="7"/>
-      <c r="D121" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="A121" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="D121" s="7"/>
       <c r="E121" s="7"/>
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>
     </row>
     <row r="122" spans="1:7">
-      <c r="A122" s="3"/>
-      <c r="B122" s="7"/>
-      <c r="C122" s="7"/>
-      <c r="D122" s="7" t="s">
-        <v>139</v>
-      </c>
+      <c r="A122" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D122" s="7"/>
       <c r="E122" s="7"/>
       <c r="F122" s="7"/>
       <c r="G122" s="7"/>
     </row>
-    <row r="123" spans="1:7">
-      <c r="A123" s="3"/>
-      <c r="B123" s="7"/>
-      <c r="C123" s="7"/>
-      <c r="D123" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E123" s="7"/>
-      <c r="F123" s="7"/>
-      <c r="G123" s="7"/>
-    </row>
     <row r="124" spans="1:7">
-      <c r="A124" s="3"/>
-      <c r="B124" s="7"/>
-      <c r="C124" s="7"/>
-      <c r="D124" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E124" s="7"/>
-      <c r="F124" s="7"/>
-      <c r="G124" s="7"/>
+      <c r="A124" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G124" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="125" spans="1:7">
-      <c r="A125" s="3"/>
-      <c r="B125" s="7"/>
-      <c r="C125" s="7"/>
-      <c r="D125" s="7" t="s">
-        <v>141</v>
-      </c>
+      <c r="A125" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="D125" s="7"/>
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
     </row>
     <row r="126" spans="1:7">
-      <c r="A126" s="3"/>
-      <c r="B126" s="7"/>
-      <c r="C126" s="7"/>
-      <c r="D126" s="7" t="s">
-        <v>141</v>
-      </c>
+      <c r="A126" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D126" s="7"/>
       <c r="E126" s="7"/>
       <c r="F126" s="7"/>
       <c r="G126" s="7"/>
     </row>
     <row r="127" spans="1:7">
-      <c r="A127" s="3"/>
-      <c r="B127" s="7"/>
-      <c r="C127" s="7"/>
-      <c r="D127" s="7" t="s">
-        <v>142</v>
-      </c>
+      <c r="A127" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D127" s="7"/>
       <c r="E127" s="7"/>
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
     </row>
     <row r="128" spans="1:7">
-      <c r="A128" s="3"/>
-      <c r="B128" s="7"/>
-      <c r="C128" s="7"/>
-      <c r="D128" s="7" t="s">
-        <v>142</v>
-      </c>
+      <c r="A128" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D128" s="7"/>
       <c r="E128" s="7"/>
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
     </row>
-    <row r="129" spans="1:7">
-      <c r="A129" s="3"/>
-      <c r="B129" s="7"/>
-      <c r="C129" s="7"/>
-      <c r="D129" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E129" s="7"/>
-      <c r="F129" s="7"/>
-      <c r="G129" s="7"/>
-    </row>
     <row r="130" spans="1:7">
-      <c r="A130" s="3"/>
-      <c r="B130" s="7"/>
-      <c r="C130" s="7"/>
-      <c r="D130" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E130" s="7"/>
-      <c r="F130" s="7"/>
-      <c r="G130" s="7"/>
+      <c r="A130" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E130" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G130" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="131" spans="1:7">
-      <c r="A131" s="3"/>
-      <c r="B131" s="7"/>
-      <c r="C131" s="7"/>
-      <c r="D131" s="7" t="s">
-        <v>144</v>
-      </c>
+      <c r="A131" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D131" s="7"/>
       <c r="E131" s="7"/>
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
     </row>
     <row r="132" spans="1:7">
-      <c r="A132" s="3"/>
-      <c r="B132" s="7"/>
-      <c r="C132" s="7"/>
-      <c r="D132" s="7" t="s">
-        <v>144</v>
-      </c>
+      <c r="A132" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D132" s="7"/>
       <c r="E132" s="7"/>
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
     </row>
     <row r="133" spans="1:7">
-      <c r="A133" s="3"/>
-      <c r="B133" s="7"/>
-      <c r="C133" s="7"/>
-      <c r="D133" s="7" t="s">
-        <v>145</v>
-      </c>
+      <c r="A133" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="D133" s="7"/>
       <c r="E133" s="7"/>
       <c r="F133" s="7"/>
       <c r="G133" s="7"/>
     </row>
     <row r="134" spans="1:7">
-      <c r="A134" s="3"/>
-      <c r="B134" s="7"/>
-      <c r="C134" s="7"/>
-      <c r="D134" s="7" t="s">
-        <v>145</v>
-      </c>
+      <c r="A134" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D134" s="7"/>
       <c r="E134" s="7"/>
       <c r="F134" s="7"/>
       <c r="G134" s="7"/>
     </row>
     <row r="135" spans="1:7">
-      <c r="A135" s="3"/>
-      <c r="B135" s="7"/>
-      <c r="C135" s="7"/>
-      <c r="D135" s="7" t="s">
-        <v>146</v>
-      </c>
+      <c r="A135" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D135" s="7"/>
       <c r="E135" s="7"/>
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
     </row>
     <row r="136" spans="1:7">
-      <c r="A136" s="3"/>
-      <c r="B136" s="7"/>
-      <c r="C136" s="7"/>
-      <c r="D136" s="7" t="s">
-        <v>146</v>
-      </c>
+      <c r="A136" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="D136" s="7"/>
       <c r="E136" s="7"/>
       <c r="F136" s="7"/>
       <c r="G136" s="7"/>
     </row>
     <row r="137" spans="1:7">
-      <c r="A137" s="3"/>
-      <c r="B137" s="7"/>
-      <c r="C137" s="7"/>
-      <c r="D137" s="7" t="s">
-        <v>147</v>
-      </c>
+      <c r="A137" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="D137" s="7"/>
       <c r="E137" s="7"/>
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
     </row>
     <row r="138" spans="1:7">
-      <c r="A138" s="3"/>
-      <c r="B138" s="7"/>
-      <c r="C138" s="7"/>
-      <c r="D138" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="A138" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="D138" s="7"/>
       <c r="E138" s="7"/>
       <c r="F138" s="7"/>
       <c r="G138" s="7"/>
     </row>
     <row r="139" spans="1:7">
-      <c r="A139" s="3"/>
-      <c r="B139" s="7"/>
-      <c r="C139" s="7"/>
-      <c r="D139" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="A139" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D139" s="7"/>
       <c r="E139" s="7"/>
       <c r="F139" s="7"/>
       <c r="G139" s="7"/>
     </row>
     <row r="140" spans="1:7">
-      <c r="A140" s="3"/>
-      <c r="B140" s="7"/>
-      <c r="C140" s="7"/>
-      <c r="D140" s="7" t="s">
-        <v>149</v>
-      </c>
+      <c r="A140" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="D140" s="7"/>
       <c r="E140" s="7"/>
       <c r="F140" s="7"/>
       <c r="G140" s="7"/>
     </row>
-    <row r="141" spans="1:7">
-      <c r="A141" s="3"/>
-      <c r="B141" s="7"/>
-      <c r="C141" s="7"/>
-      <c r="D141" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="E141" s="7"/>
-      <c r="F141" s="7"/>
-      <c r="G141" s="7"/>
-    </row>
     <row r="142" spans="1:7">
-      <c r="A142" s="3"/>
-      <c r="B142" s="7"/>
-      <c r="C142" s="7"/>
-      <c r="D142" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E142" s="7"/>
-      <c r="F142" s="7"/>
-      <c r="G142" s="7"/>
+      <c r="A142" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D142" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G142" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="143" spans="1:7">
-      <c r="A143" s="3"/>
-      <c r="B143" s="7"/>
-      <c r="C143" s="7"/>
-      <c r="D143" s="7" t="s">
-        <v>232</v>
-      </c>
+      <c r="A143" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="D143" s="7"/>
       <c r="E143" s="7"/>
       <c r="F143" s="7"/>
       <c r="G143" s="7"/>
     </row>
     <row r="144" spans="1:7">
-      <c r="A144" s="3"/>
-      <c r="B144" s="7"/>
-      <c r="C144" s="7"/>
-      <c r="D144" s="7" t="s">
-        <v>233</v>
-      </c>
+      <c r="A144" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D144" s="7"/>
       <c r="E144" s="7"/>
       <c r="F144" s="7"/>
       <c r="G144" s="7"/>
     </row>
     <row r="145" spans="1:7">
-      <c r="A145" s="3"/>
-      <c r="B145" s="7"/>
-      <c r="C145" s="7"/>
-      <c r="D145" s="7" t="s">
-        <v>234</v>
-      </c>
+      <c r="A145" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D145" s="7"/>
       <c r="E145" s="7"/>
       <c r="F145" s="7"/>
       <c r="G145" s="7"/>
     </row>
     <row r="146" spans="1:7">
-      <c r="A146" s="3"/>
-      <c r="B146" s="7"/>
-      <c r="C146" s="7"/>
-      <c r="D146" s="7" t="s">
-        <v>234</v>
-      </c>
+      <c r="A146" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C146" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="D146" s="7"/>
       <c r="E146" s="7"/>
       <c r="F146" s="7"/>
       <c r="G146" s="7"/>
     </row>
     <row r="147" spans="1:7">
-      <c r="A147" s="3"/>
-      <c r="B147" s="7"/>
-      <c r="C147" s="7"/>
-      <c r="D147" s="7" t="s">
-        <v>151</v>
-      </c>
+      <c r="A147" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="D147" s="7"/>
       <c r="E147" s="7"/>
       <c r="F147" s="7"/>
       <c r="G147" s="7"/>
     </row>
     <row r="148" spans="1:7">
-      <c r="A148" s="3"/>
-      <c r="B148" s="7"/>
-      <c r="C148" s="7"/>
-      <c r="D148" s="7" t="s">
-        <v>152</v>
-      </c>
+      <c r="A148" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C148" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="D148" s="7"/>
       <c r="E148" s="7"/>
       <c r="F148" s="7"/>
       <c r="G148" s="7"/>
     </row>
     <row r="149" spans="1:7">
-      <c r="A149" s="3"/>
-      <c r="B149" s="7"/>
-      <c r="C149" s="7"/>
-      <c r="D149" s="7" t="s">
-        <v>152</v>
-      </c>
+      <c r="A149" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D149" s="7"/>
       <c r="E149" s="7"/>
       <c r="F149" s="7"/>
       <c r="G149" s="7"/>
     </row>
     <row r="150" spans="1:7">
-      <c r="A150" s="3"/>
-      <c r="B150" s="7"/>
-      <c r="C150" s="7"/>
-      <c r="D150" s="7" t="s">
-        <v>235</v>
-      </c>
+      <c r="A150" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="D150" s="7"/>
       <c r="E150" s="7"/>
       <c r="F150" s="7"/>
       <c r="G150" s="7"/>
     </row>
     <row r="151" spans="1:7">
-      <c r="A151" s="3"/>
-      <c r="B151" s="7"/>
-      <c r="C151" s="7"/>
-      <c r="D151" s="7" t="s">
-        <v>153</v>
-      </c>
+      <c r="A151" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="D151" s="7"/>
       <c r="E151" s="7"/>
       <c r="F151" s="7"/>
       <c r="G151" s="7"/>
     </row>
     <row r="152" spans="1:7">
-      <c r="A152" s="3"/>
-      <c r="B152" s="7"/>
-      <c r="C152" s="7"/>
-      <c r="D152" s="7" t="s">
-        <v>154</v>
-      </c>
+      <c r="A152" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D152" s="7"/>
       <c r="E152" s="7"/>
       <c r="F152" s="7"/>
       <c r="G152" s="7"/>
     </row>
     <row r="153" spans="1:7">
-      <c r="A153" s="3"/>
-      <c r="B153" s="7"/>
-      <c r="C153" s="7"/>
-      <c r="D153" s="7" t="s">
-        <v>155</v>
-      </c>
+      <c r="A153" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C153" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="D153" s="7"/>
       <c r="E153" s="7"/>
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
     </row>
     <row r="154" spans="1:7">
-      <c r="A154" s="3"/>
-      <c r="B154" s="7"/>
-      <c r="C154" s="7"/>
-      <c r="D154" s="7" t="s">
-        <v>155</v>
-      </c>
+      <c r="A154" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D154" s="7"/>
       <c r="E154" s="7"/>
       <c r="F154" s="7"/>
       <c r="G154" s="7"/>
     </row>
     <row r="155" spans="1:7">
-      <c r="A155" s="3"/>
-      <c r="B155" s="7"/>
-      <c r="C155" s="7"/>
-      <c r="D155" s="7" t="s">
-        <v>156</v>
-      </c>
+      <c r="A155" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D155" s="7"/>
       <c r="E155" s="7"/>
       <c r="F155" s="7"/>
       <c r="G155" s="7"/>
     </row>
     <row r="156" spans="1:7">
-      <c r="A156" s="3"/>
-      <c r="B156" s="7"/>
-      <c r="C156" s="7"/>
-      <c r="D156" s="7" t="s">
-        <v>157</v>
-      </c>
+      <c r="A156" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D156" s="7"/>
       <c r="E156" s="7"/>
       <c r="F156" s="7"/>
       <c r="G156" s="7"/>
     </row>
-    <row r="157" spans="1:7">
-      <c r="A157" s="3"/>
-      <c r="B157" s="7"/>
-      <c r="C157" s="7"/>
-      <c r="D157" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E157" s="7"/>
-      <c r="F157" s="7"/>
-      <c r="G157" s="7"/>
-    </row>
     <row r="158" spans="1:7">
-      <c r="A158" s="3"/>
-      <c r="B158" s="7"/>
-      <c r="C158" s="7"/>
-      <c r="D158" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E158" s="7"/>
-      <c r="F158" s="7"/>
-      <c r="G158" s="7"/>
+      <c r="A158" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B158" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C158" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E158" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F158" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G158" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="159" spans="1:7">
-      <c r="A159" s="3"/>
-      <c r="B159" s="7"/>
-      <c r="C159" s="7"/>
-      <c r="D159" s="7" t="s">
-        <v>160</v>
-      </c>
+      <c r="A159" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="D159" s="7"/>
       <c r="E159" s="7"/>
       <c r="F159" s="7"/>
       <c r="G159" s="7"/>
     </row>
-    <row r="160" spans="1:7">
-      <c r="A160" s="3"/>
-      <c r="B160" s="7"/>
-      <c r="C160" s="7"/>
-      <c r="D160" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E160" s="7"/>
-      <c r="F160" s="7"/>
-      <c r="G160" s="7"/>
-    </row>
-    <row r="161" spans="1:7">
-      <c r="A161" s="3"/>
-      <c r="B161" s="7"/>
-      <c r="C161" s="7"/>
-      <c r="D161" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E161" s="7"/>
-      <c r="F161" s="7"/>
-      <c r="G161" s="7"/>
-    </row>
-    <row r="162" spans="1:7">
-      <c r="A162" s="3"/>
-      <c r="B162" s="7"/>
-      <c r="C162" s="7"/>
-      <c r="D162" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="E162" s="7"/>
-      <c r="F162" s="7"/>
-      <c r="G162" s="7"/>
-    </row>
-    <row r="163" spans="1:7">
-      <c r="A163" s="3"/>
-      <c r="B163" s="7"/>
-      <c r="C163" s="7"/>
-      <c r="D163" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E163" s="7"/>
-      <c r="F163" s="7"/>
-      <c r="G163" s="7"/>
-    </row>
-    <row r="164" spans="1:7">
-      <c r="A164" s="3"/>
-      <c r="B164" s="7"/>
-      <c r="C164" s="7"/>
-      <c r="D164" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E164" s="7"/>
-      <c r="F164" s="7"/>
-      <c r="G164" s="7"/>
-    </row>
-    <row r="165" spans="1:7">
-      <c r="A165" s="3"/>
-      <c r="B165" s="7"/>
-      <c r="C165" s="7"/>
-      <c r="D165" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="E165" s="7"/>
-      <c r="F165" s="7"/>
-      <c r="G165" s="7"/>
-    </row>
-    <row r="166" spans="1:7">
-      <c r="A166" s="3"/>
-      <c r="B166" s="7"/>
-      <c r="C166" s="7"/>
-      <c r="D166" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="E166" s="7"/>
-      <c r="F166" s="7"/>
-      <c r="G166" s="7"/>
-    </row>
-    <row r="167" spans="1:7">
-      <c r="A167" s="3"/>
-      <c r="B167" s="7"/>
-      <c r="C167" s="7"/>
-      <c r="D167" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="E167" s="7"/>
-      <c r="F167" s="7"/>
-      <c r="G167" s="7"/>
-    </row>
-    <row r="168" spans="1:7">
-      <c r="A168" s="3"/>
-      <c r="B168" s="7"/>
-      <c r="C168" s="7"/>
-      <c r="D168" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="E168" s="7"/>
-      <c r="F168" s="7"/>
-      <c r="G168" s="7"/>
-    </row>
-    <row r="169" spans="1:7">
-      <c r="A169" s="3"/>
-      <c r="B169" s="7"/>
-      <c r="C169" s="7"/>
-      <c r="D169" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="E169" s="7"/>
-      <c r="F169" s="7"/>
-      <c r="G169" s="7"/>
-    </row>
-    <row r="170" spans="1:7">
-      <c r="A170" s="3"/>
-      <c r="B170" s="7"/>
-      <c r="C170" s="7"/>
-      <c r="D170" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="E170" s="7"/>
-      <c r="F170" s="7"/>
-      <c r="G170" s="7"/>
-    </row>
-    <row r="171" spans="1:7">
-      <c r="A171" s="3"/>
-      <c r="B171" s="7"/>
-      <c r="C171" s="7"/>
-      <c r="D171" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="E171" s="7"/>
-      <c r="F171" s="7"/>
-      <c r="G171" s="7"/>
-    </row>
-    <row r="172" spans="1:7">
-      <c r="A172" s="3"/>
-      <c r="B172" s="7"/>
-      <c r="C172" s="7"/>
-      <c r="D172" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="E172" s="7"/>
-      <c r="F172" s="7"/>
-      <c r="G172" s="7"/>
-    </row>
-    <row r="173" spans="1:7">
-      <c r="A173" s="3"/>
-      <c r="B173" s="7"/>
-      <c r="C173" s="7"/>
-      <c r="D173" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E173" s="7"/>
-      <c r="F173" s="7"/>
-      <c r="G173" s="7"/>
-    </row>
-    <row r="174" spans="1:7">
-      <c r="A174" s="3"/>
-      <c r="B174" s="7"/>
-      <c r="C174" s="7"/>
-      <c r="D174" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E174" s="7"/>
-      <c r="F174" s="7"/>
-      <c r="G174" s="7"/>
-    </row>
-    <row r="175" spans="1:7">
-      <c r="A175" s="3"/>
-      <c r="B175" s="7"/>
-      <c r="C175" s="7"/>
-      <c r="D175" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E175" s="7"/>
-      <c r="F175" s="7"/>
-      <c r="G175" s="7"/>
-    </row>
-    <row r="176" spans="1:7">
-      <c r="A176" s="3"/>
-      <c r="B176" s="7"/>
-      <c r="C176" s="7"/>
-      <c r="D176" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E176" s="7"/>
-      <c r="F176" s="7"/>
-      <c r="G176" s="7"/>
-    </row>
-    <row r="177" spans="1:7">
-      <c r="A177" s="3"/>
-      <c r="B177" s="7"/>
-      <c r="C177" s="7"/>
-      <c r="D177" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E177" s="7"/>
-      <c r="F177" s="7"/>
-      <c r="G177" s="7"/>
-    </row>
-    <row r="178" spans="1:7">
-      <c r="A178" s="3"/>
-      <c r="B178" s="7"/>
-      <c r="C178" s="7"/>
-      <c r="D178" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E178" s="7"/>
-      <c r="F178" s="7"/>
-      <c r="G178" s="7"/>
-    </row>
-    <row r="179" spans="1:7">
-      <c r="A179" s="3"/>
-      <c r="B179" s="7"/>
-      <c r="C179" s="7"/>
-      <c r="D179" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E179" s="7"/>
-      <c r="F179" s="7"/>
-      <c r="G179" s="7"/>
-    </row>
-    <row r="180" spans="1:7">
-      <c r="A180" s="3"/>
-      <c r="B180" s="7"/>
-      <c r="C180" s="7"/>
-      <c r="D180" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E180" s="7"/>
-      <c r="F180" s="7"/>
-      <c r="G180" s="7"/>
-    </row>
-    <row r="181" spans="1:7">
-      <c r="A181" s="3"/>
-      <c r="B181" s="7"/>
-      <c r="C181" s="7"/>
-      <c r="D181" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E181" s="7"/>
-      <c r="F181" s="7"/>
-      <c r="G181" s="7"/>
-    </row>
-    <row r="182" spans="1:7">
-      <c r="A182" s="3"/>
-      <c r="B182" s="7"/>
-      <c r="C182" s="7"/>
-      <c r="D182" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E182" s="7"/>
-      <c r="F182" s="7"/>
-      <c r="G182" s="7"/>
-    </row>
-    <row r="183" spans="1:7">
-      <c r="A183" s="3"/>
-      <c r="B183" s="7"/>
-      <c r="C183" s="7"/>
-      <c r="D183" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E183" s="7"/>
-      <c r="F183" s="7"/>
-      <c r="G183" s="7"/>
-    </row>
-    <row r="184" spans="1:7">
-      <c r="A184" s="3"/>
-      <c r="B184" s="7"/>
-      <c r="C184" s="7"/>
-      <c r="D184" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="E184" s="7"/>
-      <c r="F184" s="7"/>
-      <c r="G184" s="7"/>
-    </row>
-    <row r="185" spans="1:7">
-      <c r="A185" s="3"/>
-      <c r="B185" s="7"/>
-      <c r="C185" s="7"/>
-      <c r="D185" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E185" s="7"/>
-      <c r="F185" s="7"/>
-      <c r="G185" s="7"/>
-    </row>
-    <row r="186" spans="1:7">
-      <c r="A186" s="3"/>
-      <c r="B186" s="7"/>
-      <c r="C186" s="7"/>
-      <c r="D186" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E186" s="7"/>
-      <c r="F186" s="7"/>
-      <c r="G186" s="7"/>
-    </row>
-    <row r="187" spans="1:7">
-      <c r="A187" s="3"/>
-      <c r="B187" s="7"/>
-      <c r="C187" s="7"/>
-      <c r="D187" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E187" s="7"/>
-      <c r="F187" s="7"/>
-      <c r="G187" s="7"/>
-    </row>
-    <row r="188" spans="1:7">
-      <c r="A188" s="3"/>
-      <c r="B188" s="7"/>
-      <c r="C188" s="7"/>
-      <c r="D188" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="E188" s="7"/>
-      <c r="F188" s="7"/>
-      <c r="G188" s="7"/>
-    </row>
-    <row r="189" spans="1:7">
-      <c r="A189" s="3"/>
-      <c r="B189" s="7"/>
-      <c r="C189" s="7"/>
-      <c r="D189" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E189" s="7"/>
-      <c r="F189" s="7"/>
-      <c r="G189" s="7"/>
-    </row>
-    <row r="190" spans="1:7">
-      <c r="A190" s="3"/>
-      <c r="B190" s="7"/>
-      <c r="C190" s="7"/>
-      <c r="D190" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="E190" s="7"/>
-      <c r="F190" s="7"/>
-      <c r="G190" s="7"/>
-    </row>
-    <row r="191" spans="1:7">
-      <c r="A191" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="B191" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C191" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="D191" s="7"/>
-      <c r="E191" s="7"/>
-      <c r="F191" s="7"/>
-      <c r="G191" s="7"/>
-    </row>
-    <row r="192" spans="1:7">
-      <c r="A192" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="B192" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="C192" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="D192" s="7"/>
-      <c r="E192" s="7"/>
-      <c r="F192" s="7"/>
-      <c r="G192" s="7"/>
-    </row>
-    <row r="193" spans="1:7">
-      <c r="A193" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="B193" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="C193" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="D193" s="7"/>
-      <c r="E193" s="7"/>
-      <c r="F193" s="7"/>
-      <c r="G193" s="7"/>
-    </row>
-    <row r="194" spans="1:7">
-      <c r="A194" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B194" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="C194" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="D194" s="7"/>
-      <c r="E194" s="7"/>
-      <c r="F194" s="7"/>
-      <c r="G194" s="7"/>
-    </row>
-    <row r="195" spans="1:7">
-      <c r="A195" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="B195" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="C195" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="D195" s="7"/>
-      <c r="E195" s="7"/>
-      <c r="F195" s="7"/>
-      <c r="G195" s="7"/>
-    </row>
-    <row r="196" spans="1:7">
-      <c r="A196" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B196" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="C196" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="D196" s="7"/>
-      <c r="E196" s="7"/>
-      <c r="F196" s="7"/>
-      <c r="G196" s="7"/>
-    </row>
-    <row r="197" spans="1:7">
-      <c r="A197" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="B197" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="C197" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="D197" s="7"/>
-      <c r="E197" s="7"/>
-      <c r="F197" s="7"/>
-      <c r="G197" s="7"/>
-    </row>
-    <row r="198" spans="1:7">
-      <c r="A198" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="B198" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="C198" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D198" s="7"/>
-      <c r="E198" s="7"/>
-      <c r="F198" s="7"/>
-      <c r="G198" s="7"/>
-    </row>
-    <row r="199" spans="1:7">
-      <c r="A199" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="B199" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="C199" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="D199" s="7"/>
-      <c r="E199" s="7"/>
-      <c r="F199" s="7"/>
-      <c r="G199" s="7"/>
-    </row>
-    <row r="200" spans="1:7">
-      <c r="A200" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B200" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="C200" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="D200" s="7"/>
-      <c r="E200" s="7"/>
-      <c r="F200" s="7"/>
-      <c r="G200" s="7"/>
-    </row>
-    <row r="201" spans="1:7">
-      <c r="A201" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="B201" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C201" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="D201" s="7"/>
-      <c r="E201" s="7"/>
-      <c r="F201" s="7"/>
-      <c r="G201" s="7"/>
-    </row>
-    <row r="202" spans="1:7">
-      <c r="A202" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="B202" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="C202" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="D202" s="7"/>
-      <c r="E202" s="7"/>
-      <c r="F202" s="7"/>
-      <c r="G202" s="7"/>
-    </row>
-    <row r="203" spans="1:7">
-      <c r="A203" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="B203" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="C203" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="D203" s="7"/>
-      <c r="E203" s="7"/>
-      <c r="F203" s="7"/>
-      <c r="G203" s="7"/>
-    </row>
-    <row r="204" spans="1:7">
-      <c r="A204" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="B204" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="C204" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="D204" s="7"/>
-      <c r="E204" s="7"/>
-      <c r="F204" s="7"/>
-      <c r="G204" s="7"/>
-    </row>
-    <row r="205" spans="1:7">
-      <c r="A205" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="B205" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="C205" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="D205" s="7"/>
-      <c r="E205" s="7"/>
-      <c r="F205" s="7"/>
-      <c r="G205" s="7"/>
-    </row>
-    <row r="206" spans="1:7">
-      <c r="A206" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="B206" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="C206" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="D206" s="7"/>
-      <c r="E206" s="7"/>
-      <c r="F206" s="7"/>
-      <c r="G206" s="7"/>
-    </row>
-    <row r="208" spans="1:7">
-      <c r="A208" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="B208" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C208" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D208" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E208" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F208" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G208" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7">
-      <c r="A209" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="B209" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="C209" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="D209" s="7"/>
-      <c r="E209" s="7"/>
-      <c r="F209" s="7"/>
-      <c r="G209" s="7"/>
-    </row>
-    <row r="210" spans="1:7">
-      <c r="A210" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="B210" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="C210" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D210" s="7"/>
-      <c r="E210" s="7"/>
-      <c r="F210" s="7"/>
-      <c r="G210" s="7"/>
-    </row>
-    <row r="212" spans="1:7">
-      <c r="A212" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="B212" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C212" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D212" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E212" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F212" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G212" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="213" spans="1:7">
-      <c r="A213" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B213" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C213" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="D213" s="7"/>
-      <c r="E213" s="7"/>
-      <c r="F213" s="7"/>
-      <c r="G213" s="7"/>
-    </row>
-    <row r="214" spans="1:7">
-      <c r="A214" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="B214" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="C214" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="D214" s="7"/>
-      <c r="E214" s="7"/>
-      <c r="F214" s="7"/>
-      <c r="G214" s="7"/>
-    </row>
-    <row r="215" spans="1:7">
-      <c r="A215" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="B215" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="C215" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="D215" s="7"/>
-      <c r="E215" s="7"/>
-      <c r="F215" s="7"/>
-      <c r="G215" s="7"/>
-    </row>
-    <row r="216" spans="1:7">
-      <c r="A216" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="B216" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="C216" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="D216" s="7"/>
-      <c r="E216" s="7"/>
-      <c r="F216" s="7"/>
-      <c r="G216" s="7"/>
-    </row>
-    <row r="218" spans="1:7">
-      <c r="A218" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="B218" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C218" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D218" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E218" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F218" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G218" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="219" spans="1:7">
-      <c r="A219" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="B219" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="C219" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="D219" s="7"/>
-      <c r="E219" s="7"/>
-      <c r="F219" s="7"/>
-      <c r="G219" s="7"/>
-    </row>
-    <row r="220" spans="1:7">
-      <c r="A220" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="B220" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C220" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="D220" s="7"/>
-      <c r="E220" s="7"/>
-      <c r="F220" s="7"/>
-      <c r="G220" s="7"/>
-    </row>
-    <row r="221" spans="1:7">
-      <c r="A221" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B221" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="C221" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="D221" s="7"/>
-      <c r="E221" s="7"/>
-      <c r="F221" s="7"/>
-      <c r="G221" s="7"/>
-    </row>
-    <row r="222" spans="1:7">
-      <c r="A222" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="B222" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="C222" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="D222" s="7"/>
-      <c r="E222" s="7"/>
-      <c r="F222" s="7"/>
-      <c r="G222" s="7"/>
-    </row>
-    <row r="223" spans="1:7">
-      <c r="A223" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="B223" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C223" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="D223" s="7"/>
-      <c r="E223" s="7"/>
-      <c r="F223" s="7"/>
-      <c r="G223" s="7"/>
-    </row>
-    <row r="224" spans="1:7">
-      <c r="A224" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="B224" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="C224" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="D224" s="7"/>
-      <c r="E224" s="7"/>
-      <c r="F224" s="7"/>
-      <c r="G224" s="7"/>
-    </row>
-    <row r="225" spans="1:7">
-      <c r="A225" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="B225" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="C225" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="D225" s="7"/>
-      <c r="E225" s="7"/>
-      <c r="F225" s="7"/>
-      <c r="G225" s="7"/>
-    </row>
-    <row r="226" spans="1:7">
-      <c r="A226" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="B226" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="C226" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="D226" s="7"/>
-      <c r="E226" s="7"/>
-      <c r="F226" s="7"/>
-      <c r="G226" s="7"/>
-    </row>
-    <row r="227" spans="1:7">
-      <c r="A227" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="B227" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="C227" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="D227" s="7"/>
-      <c r="E227" s="7"/>
-      <c r="F227" s="7"/>
-      <c r="G227" s="7"/>
-    </row>
-    <row r="228" spans="1:7">
-      <c r="A228" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="B228" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="C228" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="D228" s="7"/>
-      <c r="E228" s="7"/>
-      <c r="F228" s="7"/>
-      <c r="G228" s="7"/>
-    </row>
-    <row r="230" spans="1:7">
-      <c r="A230" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="B230" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C230" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D230" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E230" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F230" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G230" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="231" spans="1:7">
-      <c r="A231" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="B231" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="C231" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="D231" s="7"/>
-      <c r="E231" s="7"/>
-      <c r="F231" s="7"/>
-      <c r="G231" s="7"/>
-    </row>
-    <row r="232" spans="1:7">
-      <c r="A232" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="B232" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="C232" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="D232" s="7"/>
-      <c r="E232" s="7"/>
-      <c r="F232" s="7"/>
-      <c r="G232" s="7"/>
-    </row>
-    <row r="233" spans="1:7">
-      <c r="A233" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="B233" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="C233" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="D233" s="7"/>
-      <c r="E233" s="7"/>
-      <c r="F233" s="7"/>
-      <c r="G233" s="7"/>
-    </row>
-    <row r="234" spans="1:7">
-      <c r="A234" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="B234" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="C234" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="D234" s="7"/>
-      <c r="E234" s="7"/>
-      <c r="F234" s="7"/>
-      <c r="G234" s="7"/>
-    </row>
-    <row r="235" spans="1:7">
-      <c r="A235" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="B235" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="C235" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="D235" s="7"/>
-      <c r="E235" s="7"/>
-      <c r="F235" s="7"/>
-      <c r="G235" s="7"/>
-    </row>
-    <row r="236" spans="1:7">
-      <c r="A236" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="B236" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="C236" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="D236" s="7"/>
-      <c r="E236" s="7"/>
-      <c r="F236" s="7"/>
-      <c r="G236" s="7"/>
-    </row>
-    <row r="237" spans="1:7">
-      <c r="A237" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="B237" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="C237" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="D237" s="7"/>
-      <c r="E237" s="7"/>
-      <c r="F237" s="7"/>
-      <c r="G237" s="7"/>
-    </row>
-    <row r="238" spans="1:7">
-      <c r="A238" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="B238" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="C238" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="D238" s="7"/>
-      <c r="E238" s="7"/>
-      <c r="F238" s="7"/>
-      <c r="G238" s="7"/>
-    </row>
-    <row r="239" spans="1:7">
-      <c r="A239" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="B239" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="C239" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="D239" s="7"/>
-      <c r="E239" s="7"/>
-      <c r="F239" s="7"/>
-      <c r="G239" s="7"/>
-    </row>
-    <row r="240" spans="1:7">
-      <c r="A240" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="B240" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="C240" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="D240" s="7"/>
-      <c r="E240" s="7"/>
-      <c r="F240" s="7"/>
-      <c r="G240" s="7"/>
-    </row>
-    <row r="241" spans="1:7">
-      <c r="A241" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="B241" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="C241" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="D241" s="7"/>
-      <c r="E241" s="7"/>
-      <c r="F241" s="7"/>
-      <c r="G241" s="7"/>
-    </row>
-    <row r="242" spans="1:7">
-      <c r="A242" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="B242" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="C242" s="7" t="s">
-        <v>377</v>
-      </c>
-      <c r="D242" s="7"/>
-      <c r="E242" s="7"/>
-      <c r="F242" s="7"/>
-      <c r="G242" s="7"/>
-    </row>
-    <row r="243" spans="1:7">
-      <c r="A243" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B243" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="C243" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="D243" s="7"/>
-      <c r="E243" s="7"/>
-      <c r="F243" s="7"/>
-      <c r="G243" s="7"/>
-    </row>
-    <row r="244" spans="1:7">
-      <c r="A244" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="B244" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="C244" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D244" s="7"/>
-      <c r="E244" s="7"/>
-      <c r="F244" s="7"/>
-      <c r="G244" s="7"/>
-    </row>
-    <row r="246" spans="1:7">
-      <c r="A246" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="B246" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C246" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D246" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E246" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F246" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G246" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="247" spans="1:7">
-      <c r="A247" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B247" s="7" t="s">
-        <v>385</v>
-      </c>
-      <c r="C247" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="D247" s="7"/>
-      <c r="E247" s="7"/>
-      <c r="F247" s="7"/>
-      <c r="G247" s="7"/>
-    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A56:A100"/>
-    <mergeCell ref="B56:B100"/>
-    <mergeCell ref="C56:C100"/>
-    <mergeCell ref="F56:F100"/>
-    <mergeCell ref="G56:G100"/>
-    <mergeCell ref="A120:A190"/>
-    <mergeCell ref="B120:B190"/>
-    <mergeCell ref="C120:C190"/>
-    <mergeCell ref="F120:F190"/>
-    <mergeCell ref="G120:G190"/>
+    <mergeCell ref="A56:A67"/>
+    <mergeCell ref="B56:B67"/>
+    <mergeCell ref="C56:C67"/>
+    <mergeCell ref="F56:F67"/>
+    <mergeCell ref="G56:G67"/>
+    <mergeCell ref="A87:A102"/>
+    <mergeCell ref="B87:B102"/>
+    <mergeCell ref="C87:C102"/>
+    <mergeCell ref="F87:F102"/>
+    <mergeCell ref="G87:G102"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7:E247">
+  <conditionalFormatting sqref="E7:E159">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"VULN"</formula>
     </cfRule>
@@ -4822,7 +3764,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E247">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E159">
       <formula1>"PASSED,VULN"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
feat: add url and date to excel
</commit_message>
<xml_diff>
--- a/report/coba.xlsx
+++ b/report/coba.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="359">
   <si>
     <t>OWASP: Testing Guide v4.2 Checklist</t>
   </si>
   <si>
+    <t>Target URL/IP : 192.168.1.4:3000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Target Name : </t>
+  </si>
+  <si>
+    <t>Start Date : 2023-05-14</t>
   </si>
   <si>
     <t xml:space="preserve">Pentester Name : </t>
@@ -1578,61 +1584,67 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="25" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1641,13 +1653,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1656,13 +1668,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1671,13 +1683,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1686,13 +1698,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1701,13 +1713,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1716,13 +1728,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1731,13 +1743,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1746,13 +1758,13 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1761,13 +1773,13 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1776,36 +1788,36 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1814,13 +1826,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -1829,13 +1841,13 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -1844,13 +1856,13 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1859,13 +1871,13 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1874,13 +1886,13 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1889,13 +1901,13 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -1904,13 +1916,13 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -1919,13 +1931,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -1934,13 +1946,13 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -1949,13 +1961,13 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -1964,13 +1976,13 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
@@ -1979,13 +1991,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -1994,36 +2006,36 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -2032,13 +2044,13 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -2047,13 +2059,13 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -2062,13 +2074,13 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -2077,13 +2089,13 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -2092,36 +2104,36 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
@@ -2130,13 +2142,13 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
@@ -2145,13 +2157,13 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -2160,13 +2172,13 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -2175,13 +2187,13 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -2190,13 +2202,13 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -2205,13 +2217,13 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -2220,13 +2232,13 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -2235,13 +2247,13 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -2250,13 +2262,13 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
@@ -2265,36 +2277,36 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
@@ -2303,13 +2315,13 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
@@ -2318,13 +2330,13 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -2333,16 +2345,16 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
@@ -2353,7 +2365,7 @@
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
@@ -2364,7 +2376,7 @@
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
@@ -2375,7 +2387,7 @@
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
@@ -2386,7 +2398,7 @@
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
@@ -2397,7 +2409,7 @@
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
@@ -2408,7 +2420,7 @@
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
@@ -2419,7 +2431,7 @@
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
@@ -2430,7 +2442,7 @@
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
@@ -2441,7 +2453,7 @@
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
@@ -2452,7 +2464,7 @@
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
@@ -2463,7 +2475,7 @@
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
@@ -2471,13 +2483,13 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
@@ -2486,36 +2498,36 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
@@ -2524,13 +2536,13 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
@@ -2539,13 +2551,13 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
@@ -2554,13 +2566,13 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
@@ -2569,13 +2581,13 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
@@ -2584,13 +2596,13 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
@@ -2599,13 +2611,13 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
@@ -2614,13 +2626,13 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
@@ -2629,13 +2641,13 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
@@ -2644,13 +2656,13 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
@@ -2659,36 +2671,36 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
@@ -2697,13 +2709,13 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
@@ -2712,13 +2724,13 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
@@ -2727,13 +2739,13 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
@@ -2742,16 +2754,16 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
@@ -2762,7 +2774,7 @@
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
@@ -2773,7 +2785,7 @@
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
@@ -2784,7 +2796,7 @@
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
@@ -2795,7 +2807,7 @@
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
@@ -2806,7 +2818,7 @@
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E92" s="7"/>
       <c r="F92" s="7"/>
@@ -2817,7 +2829,7 @@
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
@@ -2828,7 +2840,7 @@
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
@@ -2839,7 +2851,7 @@
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
@@ -2850,7 +2862,7 @@
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
@@ -2861,7 +2873,7 @@
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
@@ -2872,7 +2884,7 @@
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
@@ -2883,7 +2895,7 @@
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
@@ -2894,7 +2906,7 @@
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
@@ -2905,7 +2917,7 @@
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
@@ -2916,7 +2928,7 @@
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
@@ -2924,13 +2936,13 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
@@ -2939,13 +2951,13 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="4" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
@@ -2954,13 +2966,13 @@
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
@@ -2969,13 +2981,13 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
@@ -2984,13 +2996,13 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="5" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
@@ -2999,13 +3011,13 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
@@ -3014,13 +3026,13 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="3" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
@@ -3029,13 +3041,13 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="4" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
@@ -3044,13 +3056,13 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
@@ -3059,13 +3071,13 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="4" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
@@ -3074,13 +3086,13 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="4" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
@@ -3089,13 +3101,13 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="5" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
@@ -3104,13 +3116,13 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
@@ -3119,13 +3131,13 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
@@ -3134,13 +3146,13 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117" s="4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
@@ -3149,13 +3161,13 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="5" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
@@ -3164,36 +3176,36 @@
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="6" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
@@ -3202,13 +3214,13 @@
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="5" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D122" s="7"/>
       <c r="E122" s="7"/>
@@ -3217,36 +3229,36 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124" s="6" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" s="5" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
@@ -3255,13 +3267,13 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126" s="5" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
@@ -3270,13 +3282,13 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="5" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D127" s="7"/>
       <c r="E127" s="7"/>
@@ -3285,13 +3297,13 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="5" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D128" s="7"/>
       <c r="E128" s="7"/>
@@ -3300,36 +3312,36 @@
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="6" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" s="4" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
@@ -3338,13 +3350,13 @@
     </row>
     <row r="132" spans="1:7">
       <c r="A132" s="5" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D132" s="7"/>
       <c r="E132" s="7"/>
@@ -3353,13 +3365,13 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="5" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>
@@ -3368,13 +3380,13 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134" s="5" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="7"/>
@@ -3383,13 +3395,13 @@
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="5" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="7"/>
@@ -3398,13 +3410,13 @@
     </row>
     <row r="136" spans="1:7">
       <c r="A136" s="5" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D136" s="7"/>
       <c r="E136" s="7"/>
@@ -3413,13 +3425,13 @@
     </row>
     <row r="137" spans="1:7">
       <c r="A137" s="5" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D137" s="7"/>
       <c r="E137" s="7"/>
@@ -3428,13 +3440,13 @@
     </row>
     <row r="138" spans="1:7">
       <c r="A138" s="5" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D138" s="7"/>
       <c r="E138" s="7"/>
@@ -3443,13 +3455,13 @@
     </row>
     <row r="139" spans="1:7">
       <c r="A139" s="4" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
@@ -3458,13 +3470,13 @@
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="4" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D140" s="7"/>
       <c r="E140" s="7"/>
@@ -3473,36 +3485,36 @@
     </row>
     <row r="142" spans="1:7">
       <c r="A142" s="6" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F142" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G142" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="143" spans="1:7">
       <c r="A143" s="4" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D143" s="7"/>
       <c r="E143" s="7"/>
@@ -3511,13 +3523,13 @@
     </row>
     <row r="144" spans="1:7">
       <c r="A144" s="5" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D144" s="7"/>
       <c r="E144" s="7"/>
@@ -3526,13 +3538,13 @@
     </row>
     <row r="145" spans="1:7">
       <c r="A145" s="5" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D145" s="7"/>
       <c r="E145" s="7"/>
@@ -3541,13 +3553,13 @@
     </row>
     <row r="146" spans="1:7">
       <c r="A146" s="5" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D146" s="7"/>
       <c r="E146" s="7"/>
@@ -3556,13 +3568,13 @@
     </row>
     <row r="147" spans="1:7">
       <c r="A147" s="5" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D147" s="7"/>
       <c r="E147" s="7"/>
@@ -3571,13 +3583,13 @@
     </row>
     <row r="148" spans="1:7">
       <c r="A148" s="5" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D148" s="7"/>
       <c r="E148" s="7"/>
@@ -3586,13 +3598,13 @@
     </row>
     <row r="149" spans="1:7">
       <c r="A149" s="5" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D149" s="7"/>
       <c r="E149" s="7"/>
@@ -3601,13 +3613,13 @@
     </row>
     <row r="150" spans="1:7">
       <c r="A150" s="5" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D150" s="7"/>
       <c r="E150" s="7"/>
@@ -3616,13 +3628,13 @@
     </row>
     <row r="151" spans="1:7">
       <c r="A151" s="5" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D151" s="7"/>
       <c r="E151" s="7"/>
@@ -3631,13 +3643,13 @@
     </row>
     <row r="152" spans="1:7">
       <c r="A152" s="5" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
@@ -3646,13 +3658,13 @@
     </row>
     <row r="153" spans="1:7">
       <c r="A153" s="5" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
@@ -3661,13 +3673,13 @@
     </row>
     <row r="154" spans="1:7">
       <c r="A154" s="5" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
@@ -3676,13 +3688,13 @@
     </row>
     <row r="155" spans="1:7">
       <c r="A155" s="5" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
@@ -3691,13 +3703,13 @@
     </row>
     <row r="156" spans="1:7">
       <c r="A156" s="5" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D156" s="7"/>
       <c r="E156" s="7"/>
@@ -3706,36 +3718,36 @@
     </row>
     <row r="158" spans="1:7">
       <c r="A158" s="6" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E158" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F158" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G158" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="159" spans="1:7">
       <c r="A159" s="4" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D159" s="7"/>
       <c r="E159" s="7"/>
@@ -3743,7 +3755,9 @@
       <c r="G159" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A56:A67"/>
     <mergeCell ref="B56:B67"/>
     <mergeCell ref="C56:C67"/>

</xml_diff>

<commit_message>
feat: update freeze column
</commit_message>
<xml_diff>
--- a/report/coba.xlsx
+++ b/report/coba.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Target Name : </t>
   </si>
   <si>
-    <t>Start Date : 2023-05-14</t>
+    <t>Start Date : 2023-05-18</t>
   </si>
   <si>
     <t xml:space="preserve">Pentester Name : </t>
@@ -1567,7 +1567,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
feat: update try catch on blank req and resp also mimetype check
</commit_message>
<xml_diff>
--- a/report/coba.xlsx
+++ b/report/coba.xlsx
@@ -14,18 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="344">
   <si>
     <t>OWASP: Testing Guide v4.2 Checklist</t>
   </si>
   <si>
-    <t>Target URL/IP : 192.168.1.4:3000</t>
+    <t>Target URL/IP : 192.168.1.14:3000</t>
   </si>
   <si>
     <t xml:space="preserve">Target Name : </t>
   </si>
   <si>
-    <t>Start Date : 2023-05-18</t>
+    <t>Start Date : 2023-05-21</t>
   </si>
   <si>
     <t xml:space="preserve">Pentester Name : </t>
@@ -436,42 +436,6 @@
     <t>- Identify injection points related to privilege manipulation.- Fuzz or otherwise attempt to bypass security measures.</t>
   </si>
   <si>
-    <t>GET http://192.168.1.4:3000/api/Addresss</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Addresss/&lt;value&gt;</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Cards</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Cards/&lt;value&gt;</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Deliverys</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Feedbacks/</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Quantitys/</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/admin/application-configuration</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/basket/&lt;value&gt;</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/captcha/</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/products/search?q=</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/user/whoami</t>
-  </si>
-  <si>
     <t>WSTG-ATHZ-04</t>
   </si>
   <si>
@@ -619,40 +583,31 @@
     <t>- Identify the backend and the parsing method used.- Assess injection points and try bypassing input filters using HPP.</t>
   </si>
   <si>
-    <t>GET http://192.168.1.4:3000/</t>
-  </si>
-  <si>
-    <t>POST http://192.168.1.4:3000/api/Addresss/</t>
-  </si>
-  <si>
-    <t>POST http://192.168.1.4:3000/api/BasketItems/</t>
-  </si>
-  <si>
-    <t>POST http://192.168.1.4:3000/api/Cards/</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Challenges/?name=&lt;value&gt;</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Deliverys/&lt;value&gt;</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/api/Products/?d=&lt;value&gt;</t>
-  </si>
-  <si>
-    <t>POST http://192.168.1.4:3000/api/SecurityAnswers/</t>
-  </si>
-  <si>
-    <t>POST http://192.168.1.4:3000/api/Users/</t>
-  </si>
-  <si>
-    <t>POST http://192.168.1.4:3000/rest/user/login</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/rest/wallet/balance</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.4:3000/socket.io/?EIO=&lt;value&gt;&amp;transport=&lt;value&gt;&amp;t=&lt;value&gt;&amp;sid=&lt;value&gt;</t>
+    <t>GET http://192.168.1.14:3000/socket.io/?EIO=&lt;value&gt;&amp;transport=&lt;value&gt;&amp;t=&lt;value&gt;&amp;sid=&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.14:3000/rest/admin/application-configuration</t>
+  </si>
+  <si>
+    <t>POST http://192.168.1.14:3000/api/Users/</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.14:3000/font-mfizz.woff</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.14:3000/rest/user/whoami</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.14:3000/rest/products/search?q=</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.14:3000/api/Challenges/?name=&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.14:3000/rest/languages</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.14:3000/</t>
   </si>
   <si>
     <t>WSTG-INPV-05</t>
@@ -1565,7 +1520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G159"/>
+  <dimension ref="A1:G140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
@@ -2333,13 +2288,13 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="4" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -2347,152 +2302,187 @@
       <c r="G55" s="7"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="4" t="s">
-        <v>152</v>
+      <c r="A56" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>140</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="4"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-    </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="4"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
+      <c r="A58" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="4"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7" t="s">
-        <v>143</v>
-      </c>
+      <c r="A59" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D59" s="7"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="4"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7" t="s">
-        <v>144</v>
-      </c>
+      <c r="A60" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="4"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7" t="s">
-        <v>145</v>
-      </c>
+      <c r="A61" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="4"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7" t="s">
-        <v>146</v>
-      </c>
+      <c r="A62" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D62" s="7"/>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="4"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7" t="s">
-        <v>147</v>
-      </c>
+      <c r="A63" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D63" s="7"/>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="4"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="A64" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="4"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7" t="s">
-        <v>149</v>
-      </c>
+      <c r="A65" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D65" s="7"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="4"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7" t="s">
-        <v>150</v>
-      </c>
+      <c r="A66" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D66" s="7"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="4"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7" t="s">
-        <v>151</v>
-      </c>
+      <c r="A67" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="5" t="s">
-        <v>155</v>
+      <c r="A68" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
@@ -2501,7 +2491,7 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="6" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>10</v>
@@ -2524,13 +2514,13 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="5" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
@@ -2538,14 +2528,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="5" t="s">
-        <v>162</v>
+      <c r="A72" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
@@ -2554,13 +2544,13 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="5" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>167</v>
+        <v>41</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
@@ -2569,13 +2559,13 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="5" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
@@ -2583,142 +2573,119 @@
       <c r="G74" s="7"/>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="5" t="s">
-        <v>171</v>
+      <c r="A75" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>172</v>
+        <v>199</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D75" s="7"/>
+        <v>200</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>189</v>
+      </c>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D76" s="7"/>
+      <c r="A76" s="3"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7" t="s">
+        <v>190</v>
+      </c>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D77" s="7"/>
+      <c r="A77" s="3"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7" t="s">
+        <v>191</v>
+      </c>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D78" s="7"/>
+      <c r="A78" s="3"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7" t="s">
+        <v>192</v>
+      </c>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D79" s="7"/>
+      <c r="A79" s="3"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D80" s="7"/>
+      <c r="A80" s="3"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7" t="s">
+        <v>194</v>
+      </c>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
     </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="3"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+    </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A82" s="3"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D83" s="7"/>
+      <c r="A83" s="3"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7" t="s">
+        <v>197</v>
+      </c>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="4" t="s">
-        <v>193</v>
+      <c r="A84" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
@@ -2726,14 +2693,14 @@
       <c r="G84" s="7"/>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="5" t="s">
-        <v>196</v>
+      <c r="A85" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>41</v>
+        <v>206</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
@@ -2741,14 +2708,14 @@
       <c r="G85" s="7"/>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="5" t="s">
-        <v>198</v>
+      <c r="A86" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
@@ -2756,241 +2723,285 @@
       <c r="G86" s="7"/>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="3" t="s">
-        <v>213</v>
+      <c r="A87" s="4" t="s">
+        <v>210</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>201</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
     </row>
     <row r="88" spans="1:7">
-      <c r="A88" s="3"/>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="7" t="s">
-        <v>202</v>
-      </c>
+      <c r="A88" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D88" s="7"/>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="3"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
-      <c r="D89" s="7" t="s">
-        <v>203</v>
-      </c>
+      <c r="A89" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D89" s="7"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="3"/>
-      <c r="B90" s="7"/>
-      <c r="C90" s="7"/>
-      <c r="D90" s="7" t="s">
-        <v>204</v>
-      </c>
+      <c r="A90" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D90" s="7"/>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="3"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="7" t="s">
-        <v>205</v>
-      </c>
+      <c r="A91" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D91" s="7"/>
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
     </row>
     <row r="92" spans="1:7">
-      <c r="A92" s="3"/>
-      <c r="B92" s="7"/>
-      <c r="C92" s="7"/>
-      <c r="D92" s="7" t="s">
-        <v>206</v>
-      </c>
+      <c r="A92" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D92" s="7"/>
       <c r="E92" s="7"/>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
     </row>
     <row r="93" spans="1:7">
-      <c r="A93" s="3"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7" t="s">
-        <v>207</v>
-      </c>
+      <c r="A93" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D93" s="7"/>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
     </row>
     <row r="94" spans="1:7">
-      <c r="A94" s="3"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7" t="s">
-        <v>208</v>
-      </c>
+      <c r="A94" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D94" s="7"/>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
     </row>
     <row r="95" spans="1:7">
-      <c r="A95" s="3"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7" t="s">
-        <v>209</v>
-      </c>
+      <c r="A95" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D95" s="7"/>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
     </row>
     <row r="96" spans="1:7">
-      <c r="A96" s="3"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7" t="s">
-        <v>147</v>
-      </c>
+      <c r="A96" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D96" s="7"/>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="3"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="7"/>
-      <c r="D97" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="A97" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D97" s="7"/>
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
     </row>
     <row r="98" spans="1:7">
-      <c r="A98" s="3"/>
-      <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="7" t="s">
-        <v>149</v>
-      </c>
+      <c r="A98" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="D98" s="7"/>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
     </row>
     <row r="99" spans="1:7">
-      <c r="A99" s="3"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="7" t="s">
-        <v>150</v>
-      </c>
+      <c r="A99" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D99" s="7"/>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
     </row>
-    <row r="100" spans="1:7">
-      <c r="A100" s="3"/>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E100" s="7"/>
-      <c r="F100" s="7"/>
-      <c r="G100" s="7"/>
-    </row>
     <row r="101" spans="1:7">
-      <c r="A101" s="3"/>
-      <c r="B101" s="7"/>
-      <c r="C101" s="7"/>
-      <c r="D101" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E101" s="7"/>
-      <c r="F101" s="7"/>
-      <c r="G101" s="7"/>
+      <c r="A101" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G101" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="102" spans="1:7">
-      <c r="A102" s="3"/>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7" t="s">
-        <v>212</v>
-      </c>
+      <c r="A102" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D102" s="7"/>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
     </row>
     <row r="103" spans="1:7">
-      <c r="A103" s="3" t="s">
-        <v>216</v>
+      <c r="A103" s="5" t="s">
+        <v>252</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>217</v>
+        <v>253</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>218</v>
+        <v>41</v>
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
     </row>
-    <row r="104" spans="1:7">
-      <c r="A104" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="D104" s="7"/>
-      <c r="E104" s="7"/>
-      <c r="F104" s="7"/>
-      <c r="G104" s="7"/>
-    </row>
     <row r="105" spans="1:7">
-      <c r="A105" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="D105" s="7"/>
-      <c r="E105" s="7"/>
-      <c r="F105" s="7"/>
-      <c r="G105" s="7"/>
+      <c r="A105" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="106" spans="1:7">
-      <c r="A106" s="4" t="s">
-        <v>225</v>
+      <c r="A106" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>227</v>
+        <v>257</v>
       </c>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
@@ -2999,13 +3010,13 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="5" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>230</v>
+        <v>260</v>
       </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
@@ -3013,14 +3024,14 @@
       <c r="G107" s="7"/>
     </row>
     <row r="108" spans="1:7">
-      <c r="A108" s="3" t="s">
-        <v>231</v>
+      <c r="A108" s="5" t="s">
+        <v>261</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>232</v>
+        <v>262</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
@@ -3028,59 +3039,52 @@
       <c r="G108" s="7"/>
     </row>
     <row r="109" spans="1:7">
-      <c r="A109" s="3" t="s">
-        <v>234</v>
+      <c r="A109" s="5" t="s">
+        <v>264</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>235</v>
+        <v>265</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>236</v>
+        <v>266</v>
       </c>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
     </row>
-    <row r="110" spans="1:7">
-      <c r="A110" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D110" s="7"/>
-      <c r="E110" s="7"/>
-      <c r="F110" s="7"/>
-      <c r="G110" s="7"/>
-    </row>
     <row r="111" spans="1:7">
-      <c r="A111" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="D111" s="7"/>
-      <c r="E111" s="7"/>
-      <c r="F111" s="7"/>
-      <c r="G111" s="7"/>
+      <c r="A111" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="4" t="s">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>243</v>
+        <v>269</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>244</v>
+        <v>270</v>
       </c>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
@@ -3088,14 +3092,14 @@
       <c r="G112" s="7"/>
     </row>
     <row r="113" spans="1:7">
-      <c r="A113" s="4" t="s">
-        <v>245</v>
+      <c r="A113" s="5" t="s">
+        <v>271</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>246</v>
+        <v>272</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>247</v>
+        <v>273</v>
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
@@ -3104,13 +3108,13 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="5" t="s">
-        <v>248</v>
+        <v>274</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>249</v>
+        <v>275</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>250</v>
+        <v>276</v>
       </c>
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
@@ -3118,14 +3122,14 @@
       <c r="G114" s="7"/>
     </row>
     <row r="115" spans="1:7">
-      <c r="A115" s="4" t="s">
-        <v>251</v>
+      <c r="A115" s="5" t="s">
+        <v>277</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
@@ -3133,14 +3137,14 @@
       <c r="G115" s="7"/>
     </row>
     <row r="116" spans="1:7">
-      <c r="A116" s="3" t="s">
-        <v>254</v>
+      <c r="A116" s="5" t="s">
+        <v>280</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>255</v>
+        <v>281</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>256</v>
+        <v>282</v>
       </c>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
@@ -3148,14 +3152,14 @@
       <c r="G116" s="7"/>
     </row>
     <row r="117" spans="1:7">
-      <c r="A117" s="4" t="s">
-        <v>257</v>
+      <c r="A117" s="5" t="s">
+        <v>283</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>259</v>
+        <v>285</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
@@ -3164,104 +3168,111 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="5" t="s">
-        <v>260</v>
+        <v>286</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>261</v>
+        <v>287</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>262</v>
+        <v>288</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
       <c r="F118" s="7"/>
       <c r="G118" s="7"/>
     </row>
+    <row r="119" spans="1:7">
+      <c r="A119" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
+      <c r="F119" s="7"/>
+      <c r="G119" s="7"/>
+    </row>
     <row r="120" spans="1:7">
-      <c r="A120" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E120" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F120" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G120" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A120" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="D120" s="7"/>
+      <c r="E120" s="7"/>
+      <c r="F120" s="7"/>
+      <c r="G120" s="7"/>
     </row>
     <row r="121" spans="1:7">
-      <c r="A121" s="5" t="s">
-        <v>264</v>
+      <c r="A121" s="4" t="s">
+        <v>295</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>265</v>
+        <v>296</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>
     </row>
-    <row r="122" spans="1:7">
-      <c r="A122" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="B122" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D122" s="7"/>
-      <c r="E122" s="7"/>
-      <c r="F122" s="7"/>
-      <c r="G122" s="7"/>
+    <row r="123" spans="1:7">
+      <c r="A123" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F123" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G123" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="124" spans="1:7">
-      <c r="A124" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D124" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E124" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F124" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G124" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A124" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="D124" s="7"/>
+      <c r="E124" s="7"/>
+      <c r="F124" s="7"/>
+      <c r="G124" s="7"/>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" s="5" t="s">
-        <v>270</v>
+        <v>302</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>271</v>
+        <v>303</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>272</v>
+        <v>304</v>
       </c>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
@@ -3270,13 +3281,13 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126" s="5" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>274</v>
+        <v>306</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>275</v>
+        <v>307</v>
       </c>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
@@ -3285,13 +3296,13 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="5" t="s">
-        <v>276</v>
+        <v>308</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>277</v>
+        <v>309</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>278</v>
+        <v>310</v>
       </c>
       <c r="D127" s="7"/>
       <c r="E127" s="7"/>
@@ -3300,51 +3311,58 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="5" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>280</v>
+        <v>312</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>281</v>
+        <v>313</v>
       </c>
       <c r="D128" s="7"/>
       <c r="E128" s="7"/>
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
     </row>
+    <row r="129" spans="1:7">
+      <c r="A129" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D129" s="7"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7"/>
+      <c r="G129" s="7"/>
+    </row>
     <row r="130" spans="1:7">
-      <c r="A130" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="B130" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E130" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F130" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G130" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A130" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="D130" s="7"/>
+      <c r="E130" s="7"/>
+      <c r="F130" s="7"/>
+      <c r="G130" s="7"/>
     </row>
     <row r="131" spans="1:7">
-      <c r="A131" s="4" t="s">
-        <v>283</v>
+      <c r="A131" s="5" t="s">
+        <v>320</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>284</v>
+        <v>321</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>285</v>
+        <v>322</v>
       </c>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
@@ -3353,13 +3371,13 @@
     </row>
     <row r="132" spans="1:7">
       <c r="A132" s="5" t="s">
-        <v>286</v>
+        <v>323</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>287</v>
+        <v>324</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>288</v>
+        <v>325</v>
       </c>
       <c r="D132" s="7"/>
       <c r="E132" s="7"/>
@@ -3368,13 +3386,13 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="5" t="s">
-        <v>289</v>
+        <v>326</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>290</v>
+        <v>327</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>291</v>
+        <v>328</v>
       </c>
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>
@@ -3383,13 +3401,13 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134" s="5" t="s">
-        <v>292</v>
+        <v>329</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>293</v>
+        <v>330</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>294</v>
+        <v>331</v>
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="7"/>
@@ -3398,13 +3416,13 @@
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="5" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>296</v>
+        <v>333</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>297</v>
+        <v>334</v>
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="7"/>
@@ -3413,13 +3431,13 @@
     </row>
     <row r="136" spans="1:7">
       <c r="A136" s="5" t="s">
-        <v>298</v>
+        <v>335</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>299</v>
+        <v>336</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>300</v>
+        <v>337</v>
       </c>
       <c r="D136" s="7"/>
       <c r="E136" s="7"/>
@@ -3428,351 +3446,73 @@
     </row>
     <row r="137" spans="1:7">
       <c r="A137" s="5" t="s">
-        <v>301</v>
+        <v>338</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>302</v>
+        <v>339</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>303</v>
+        <v>41</v>
       </c>
       <c r="D137" s="7"/>
       <c r="E137" s="7"/>
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
     </row>
-    <row r="138" spans="1:7">
-      <c r="A138" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="B138" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="C138" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="D138" s="7"/>
-      <c r="E138" s="7"/>
-      <c r="F138" s="7"/>
-      <c r="G138" s="7"/>
-    </row>
     <row r="139" spans="1:7">
-      <c r="A139" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B139" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="C139" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="D139" s="7"/>
-      <c r="E139" s="7"/>
-      <c r="F139" s="7"/>
-      <c r="G139" s="7"/>
+      <c r="A139" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D139" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F139" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G139" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="4" t="s">
-        <v>310</v>
+        <v>341</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>311</v>
+        <v>342</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>312</v>
+        <v>343</v>
       </c>
       <c r="D140" s="7"/>
       <c r="E140" s="7"/>
       <c r="F140" s="7"/>
       <c r="G140" s="7"/>
     </row>
-    <row r="142" spans="1:7">
-      <c r="A142" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="B142" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D142" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E142" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F142" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G142" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7">
-      <c r="A143" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="B143" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C143" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="D143" s="7"/>
-      <c r="E143" s="7"/>
-      <c r="F143" s="7"/>
-      <c r="G143" s="7"/>
-    </row>
-    <row r="144" spans="1:7">
-      <c r="A144" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B144" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="C144" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="D144" s="7"/>
-      <c r="E144" s="7"/>
-      <c r="F144" s="7"/>
-      <c r="G144" s="7"/>
-    </row>
-    <row r="145" spans="1:7">
-      <c r="A145" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="B145" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="C145" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="D145" s="7"/>
-      <c r="E145" s="7"/>
-      <c r="F145" s="7"/>
-      <c r="G145" s="7"/>
-    </row>
-    <row r="146" spans="1:7">
-      <c r="A146" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="B146" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C146" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="D146" s="7"/>
-      <c r="E146" s="7"/>
-      <c r="F146" s="7"/>
-      <c r="G146" s="7"/>
-    </row>
-    <row r="147" spans="1:7">
-      <c r="A147" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="B147" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="C147" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="D147" s="7"/>
-      <c r="E147" s="7"/>
-      <c r="F147" s="7"/>
-      <c r="G147" s="7"/>
-    </row>
-    <row r="148" spans="1:7">
-      <c r="A148" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="B148" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="D148" s="7"/>
-      <c r="E148" s="7"/>
-      <c r="F148" s="7"/>
-      <c r="G148" s="7"/>
-    </row>
-    <row r="149" spans="1:7">
-      <c r="A149" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="B149" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="C149" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="D149" s="7"/>
-      <c r="E149" s="7"/>
-      <c r="F149" s="7"/>
-      <c r="G149" s="7"/>
-    </row>
-    <row r="150" spans="1:7">
-      <c r="A150" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="B150" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="C150" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="D150" s="7"/>
-      <c r="E150" s="7"/>
-      <c r="F150" s="7"/>
-      <c r="G150" s="7"/>
-    </row>
-    <row r="151" spans="1:7">
-      <c r="A151" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="B151" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="C151" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="D151" s="7"/>
-      <c r="E151" s="7"/>
-      <c r="F151" s="7"/>
-      <c r="G151" s="7"/>
-    </row>
-    <row r="152" spans="1:7">
-      <c r="A152" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="B152" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="D152" s="7"/>
-      <c r="E152" s="7"/>
-      <c r="F152" s="7"/>
-      <c r="G152" s="7"/>
-    </row>
-    <row r="153" spans="1:7">
-      <c r="A153" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="B153" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="C153" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="D153" s="7"/>
-      <c r="E153" s="7"/>
-      <c r="F153" s="7"/>
-      <c r="G153" s="7"/>
-    </row>
-    <row r="154" spans="1:7">
-      <c r="A154" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="B154" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="C154" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="D154" s="7"/>
-      <c r="E154" s="7"/>
-      <c r="F154" s="7"/>
-      <c r="G154" s="7"/>
-    </row>
-    <row r="155" spans="1:7">
-      <c r="A155" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="B155" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="C155" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="D155" s="7"/>
-      <c r="E155" s="7"/>
-      <c r="F155" s="7"/>
-      <c r="G155" s="7"/>
-    </row>
-    <row r="156" spans="1:7">
-      <c r="A156" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="B156" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="C156" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D156" s="7"/>
-      <c r="E156" s="7"/>
-      <c r="F156" s="7"/>
-      <c r="G156" s="7"/>
-    </row>
-    <row r="158" spans="1:7">
-      <c r="A158" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="B158" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C158" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D158" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E158" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F158" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G158" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7">
-      <c r="A159" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="B159" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="C159" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="D159" s="7"/>
-      <c r="E159" s="7"/>
-      <c r="F159" s="7"/>
-      <c r="G159" s="7"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A56:A67"/>
-    <mergeCell ref="B56:B67"/>
-    <mergeCell ref="C56:C67"/>
-    <mergeCell ref="F56:F67"/>
-    <mergeCell ref="G56:G67"/>
-    <mergeCell ref="A87:A102"/>
-    <mergeCell ref="B87:B102"/>
-    <mergeCell ref="C87:C102"/>
-    <mergeCell ref="F87:F102"/>
-    <mergeCell ref="G87:G102"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="A75:A83"/>
+    <mergeCell ref="B75:B83"/>
+    <mergeCell ref="C75:C83"/>
+    <mergeCell ref="F75:F83"/>
+    <mergeCell ref="G75:G83"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7:E159">
+  <conditionalFormatting sqref="E7:E140">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"VULN"</formula>
     </cfRule>
@@ -3781,7 +3521,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E159">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E140">
       <formula1>"PASSED,VULN"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
feat: update type report arguments
</commit_message>
<xml_diff>
--- a/report/coba.xlsx
+++ b/report/coba.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="335">
   <si>
     <t>OWASP: Testing Guide v4.2 Checklist</t>
   </si>
@@ -581,33 +581,6 @@
   </si>
   <si>
     <t>- Identify the backend and the parsing method used.- Assess injection points and try bypassing input filters using HPP.</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.14:3000/socket.io/?EIO=&lt;value&gt;&amp;transport=&lt;value&gt;&amp;t=&lt;value&gt;&amp;sid=&lt;value&gt;</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.14:3000/rest/admin/application-configuration</t>
-  </si>
-  <si>
-    <t>POST http://192.168.1.14:3000/api/Users/</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.14:3000/font-mfizz.woff</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.14:3000/rest/user/whoami</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.14:3000/rest/products/search?q=</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.14:3000/api/Challenges/?name=&lt;value&gt;</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.14:3000/rest/languages</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.14:3000/</t>
   </si>
   <si>
     <t>WSTG-INPV-05</t>
@@ -1520,7 +1493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G140"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
@@ -2558,14 +2531,14 @@
       <c r="G73" s="7"/>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="5" t="s">
-        <v>186</v>
+      <c r="A74" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
@@ -2574,118 +2547,148 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>189</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="D75" s="7"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="3"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7" t="s">
-        <v>190</v>
-      </c>
+      <c r="A76" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="3"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7" t="s">
-        <v>191</v>
-      </c>
+      <c r="A77" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D77" s="7"/>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="3"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7" t="s">
-        <v>192</v>
-      </c>
+      <c r="A78" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="3"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7" t="s">
-        <v>193</v>
-      </c>
+      <c r="A79" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D79" s="7"/>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="3"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7" t="s">
-        <v>194</v>
-      </c>
+      <c r="A80" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D80" s="7"/>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="3"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
-      <c r="D81" s="7" t="s">
-        <v>195</v>
-      </c>
+      <c r="A81" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D81" s="7"/>
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="3"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7" t="s">
-        <v>196</v>
-      </c>
+      <c r="A82" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D82" s="7"/>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="3"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="7" t="s">
-        <v>197</v>
-      </c>
+      <c r="A83" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D83" s="7"/>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="3" t="s">
-        <v>201</v>
+      <c r="A84" s="4" t="s">
+        <v>218</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
@@ -2694,13 +2697,13 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="4" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
@@ -2708,14 +2711,14 @@
       <c r="G85" s="7"/>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="3" t="s">
-        <v>207</v>
+      <c r="A86" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
@@ -2724,13 +2727,13 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="4" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
@@ -2738,14 +2741,14 @@
       <c r="G87" s="7"/>
     </row>
     <row r="88" spans="1:7">
-      <c r="A88" s="5" t="s">
-        <v>213</v>
+      <c r="A88" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
@@ -2753,14 +2756,14 @@
       <c r="G88" s="7"/>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="3" t="s">
-        <v>216</v>
+      <c r="A89" s="4" t="s">
+        <v>233</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
@@ -2768,59 +2771,52 @@
       <c r="G89" s="7"/>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="3" t="s">
-        <v>219</v>
+      <c r="A90" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
     </row>
-    <row r="91" spans="1:7">
-      <c r="A91" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
-      <c r="F91" s="7"/>
-      <c r="G91" s="7"/>
-    </row>
     <row r="92" spans="1:7">
-      <c r="A92" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D92" s="7"/>
-      <c r="E92" s="7"/>
-      <c r="F92" s="7"/>
-      <c r="G92" s="7"/>
+      <c r="A92" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G92" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="93" spans="1:7">
-      <c r="A93" s="4" t="s">
-        <v>227</v>
+      <c r="A93" s="5" t="s">
+        <v>240</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
@@ -2828,59 +2824,52 @@
       <c r="G93" s="7"/>
     </row>
     <row r="94" spans="1:7">
-      <c r="A94" s="4" t="s">
-        <v>230</v>
+      <c r="A94" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>232</v>
+        <v>41</v>
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
     </row>
-    <row r="95" spans="1:7">
-      <c r="A95" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
-      <c r="F95" s="7"/>
-      <c r="G95" s="7"/>
-    </row>
     <row r="96" spans="1:7">
-      <c r="A96" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="B96" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D96" s="7"/>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
-      <c r="G96" s="7"/>
+      <c r="A96" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="3" t="s">
-        <v>239</v>
+      <c r="A97" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
@@ -2888,14 +2877,14 @@
       <c r="G97" s="7"/>
     </row>
     <row r="98" spans="1:7">
-      <c r="A98" s="4" t="s">
-        <v>242</v>
+      <c r="A98" s="5" t="s">
+        <v>249</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
@@ -2904,104 +2893,111 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="5" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
     </row>
-    <row r="101" spans="1:7">
-      <c r="A101" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="B101" s="6" t="s">
+    <row r="100" spans="1:7">
+      <c r="A100" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C101" s="6" t="s">
+      <c r="C102" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D101" s="6" t="s">
+      <c r="D102" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E101" s="6" t="s">
+      <c r="E102" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F101" s="6" t="s">
+      <c r="F102" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G101" s="6" t="s">
+      <c r="G102" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
-      <c r="A102" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="D102" s="7"/>
-      <c r="E102" s="7"/>
-      <c r="F102" s="7"/>
-      <c r="G102" s="7"/>
-    </row>
     <row r="103" spans="1:7">
-      <c r="A103" s="5" t="s">
-        <v>252</v>
+      <c r="A103" s="4" t="s">
+        <v>259</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>41</v>
+        <v>261</v>
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
     </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
+      <c r="G104" s="7"/>
+    </row>
     <row r="105" spans="1:7">
-      <c r="A105" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E105" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A105" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="7"/>
+      <c r="G105" s="7"/>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="5" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
@@ -3010,13 +3006,13 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="5" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
@@ -3025,13 +3021,13 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="5" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
@@ -3040,96 +3036,96 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="5" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
     </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D110" s="7"/>
+      <c r="E110" s="7"/>
+      <c r="F110" s="7"/>
+      <c r="G110" s="7"/>
+    </row>
     <row r="111" spans="1:7">
-      <c r="A111" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E111" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F111" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G111" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A111" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7"/>
+      <c r="G111" s="7"/>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="4" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
     </row>
-    <row r="113" spans="1:7">
-      <c r="A113" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="B113" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C113" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
-      <c r="F113" s="7"/>
-      <c r="G113" s="7"/>
-    </row>
     <row r="114" spans="1:7">
-      <c r="A114" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="B114" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="D114" s="7"/>
-      <c r="E114" s="7"/>
-      <c r="F114" s="7"/>
-      <c r="G114" s="7"/>
+      <c r="A114" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F114" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G114" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="115" spans="1:7">
-      <c r="A115" s="5" t="s">
-        <v>277</v>
+      <c r="A115" s="4" t="s">
+        <v>290</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
@@ -3138,13 +3134,13 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="5" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
@@ -3153,13 +3149,13 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117" s="5" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
@@ -3168,13 +3164,13 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="5" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
@@ -3183,13 +3179,13 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="5" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>291</v>
+        <v>304</v>
       </c>
       <c r="D119" s="7"/>
       <c r="E119" s="7"/>
@@ -3197,14 +3193,14 @@
       <c r="G119" s="7"/>
     </row>
     <row r="120" spans="1:7">
-      <c r="A120" s="4" t="s">
-        <v>292</v>
+      <c r="A120" s="5" t="s">
+        <v>305</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="D120" s="7"/>
       <c r="E120" s="7"/>
@@ -3212,52 +3208,59 @@
       <c r="G120" s="7"/>
     </row>
     <row r="121" spans="1:7">
-      <c r="A121" s="4" t="s">
-        <v>295</v>
+      <c r="A121" s="5" t="s">
+        <v>308</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>
     </row>
+    <row r="122" spans="1:7">
+      <c r="A122" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="D122" s="7"/>
+      <c r="E122" s="7"/>
+      <c r="F122" s="7"/>
+      <c r="G122" s="7"/>
+    </row>
     <row r="123" spans="1:7">
-      <c r="A123" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D123" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E123" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F123" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G123" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A123" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7"/>
+      <c r="G123" s="7"/>
     </row>
     <row r="124" spans="1:7">
-      <c r="A124" s="4" t="s">
-        <v>299</v>
+      <c r="A124" s="5" t="s">
+        <v>317</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
@@ -3266,13 +3269,13 @@
     </row>
     <row r="125" spans="1:7">
       <c r="A125" s="5" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>303</v>
+        <v>321</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
@@ -3281,13 +3284,13 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126" s="5" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>307</v>
+        <v>325</v>
       </c>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
@@ -3296,13 +3299,13 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="5" t="s">
-        <v>308</v>
+        <v>326</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>310</v>
+        <v>328</v>
       </c>
       <c r="D127" s="7"/>
       <c r="E127" s="7"/>
@@ -3311,191 +3314,56 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="5" t="s">
-        <v>311</v>
+        <v>329</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>312</v>
+        <v>330</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>313</v>
+        <v>41</v>
       </c>
       <c r="D128" s="7"/>
       <c r="E128" s="7"/>
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
     </row>
-    <row r="129" spans="1:7">
-      <c r="A129" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="B129" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="D129" s="7"/>
-      <c r="E129" s="7"/>
-      <c r="F129" s="7"/>
-      <c r="G129" s="7"/>
-    </row>
     <row r="130" spans="1:7">
-      <c r="A130" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="C130" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="D130" s="7"/>
-      <c r="E130" s="7"/>
-      <c r="F130" s="7"/>
-      <c r="G130" s="7"/>
+      <c r="A130" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E130" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G130" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="131" spans="1:7">
-      <c r="A131" s="5" t="s">
-        <v>320</v>
+      <c r="A131" s="4" t="s">
+        <v>332</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
-    </row>
-    <row r="132" spans="1:7">
-      <c r="A132" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="B132" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C132" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="D132" s="7"/>
-      <c r="E132" s="7"/>
-      <c r="F132" s="7"/>
-      <c r="G132" s="7"/>
-    </row>
-    <row r="133" spans="1:7">
-      <c r="A133" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="D133" s="7"/>
-      <c r="E133" s="7"/>
-      <c r="F133" s="7"/>
-      <c r="G133" s="7"/>
-    </row>
-    <row r="134" spans="1:7">
-      <c r="A134" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="B134" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="D134" s="7"/>
-      <c r="E134" s="7"/>
-      <c r="F134" s="7"/>
-      <c r="G134" s="7"/>
-    </row>
-    <row r="135" spans="1:7">
-      <c r="A135" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="B135" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="C135" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="D135" s="7"/>
-      <c r="E135" s="7"/>
-      <c r="F135" s="7"/>
-      <c r="G135" s="7"/>
-    </row>
-    <row r="136" spans="1:7">
-      <c r="A136" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="B136" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="D136" s="7"/>
-      <c r="E136" s="7"/>
-      <c r="F136" s="7"/>
-      <c r="G136" s="7"/>
-    </row>
-    <row r="137" spans="1:7">
-      <c r="A137" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="B137" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D137" s="7"/>
-      <c r="E137" s="7"/>
-      <c r="F137" s="7"/>
-      <c r="G137" s="7"/>
-    </row>
-    <row r="139" spans="1:7">
-      <c r="A139" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="B139" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C139" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D139" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E139" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F139" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G139" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7">
-      <c r="A140" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="B140" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="C140" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="D140" s="7"/>
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
-      <c r="G140" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3506,13 +3374,13 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="F55:F56"/>
     <mergeCell ref="G55:G56"/>
-    <mergeCell ref="A75:A83"/>
-    <mergeCell ref="B75:B83"/>
-    <mergeCell ref="C75:C83"/>
-    <mergeCell ref="F75:F83"/>
-    <mergeCell ref="G75:G83"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="G74:G75"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7:E140">
+  <conditionalFormatting sqref="E7:E131">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"VULN"</formula>
     </cfRule>
@@ -3521,7 +3389,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E140">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E131">
       <formula1>"PASSED,VULN"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
feat: add type detail for report
</commit_message>
<xml_diff>
--- a/report/coba.xlsx
+++ b/report/coba.xlsx
@@ -14,18 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="359">
   <si>
     <t>OWASP: Testing Guide v4.2 Checklist</t>
   </si>
   <si>
-    <t>Target URL/IP : 192.168.1.14:3000</t>
+    <t>Target URL/IP : 192.168.1.4:3000</t>
   </si>
   <si>
     <t xml:space="preserve">Target Name : </t>
   </si>
   <si>
-    <t>Start Date : 2023-05-21</t>
+    <t>Start Date : 2023-05-22</t>
   </si>
   <si>
     <t xml:space="preserve">Pentester Name : </t>
@@ -436,6 +436,42 @@
     <t>- Identify injection points related to privilege manipulation.- Fuzz or otherwise attempt to bypass security measures.</t>
   </si>
   <si>
+    <t>GET http://192.168.1.4:3000/api/Addresss</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Addresss/&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Cards</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Cards/&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Deliverys</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Feedbacks/</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Quantitys/</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/rest/admin/application-configuration</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/rest/basket/&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/rest/captcha/</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/rest/products/search?q=</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/rest/user/whoami</t>
+  </si>
+  <si>
     <t>WSTG-ATHZ-04</t>
   </si>
   <si>
@@ -581,6 +617,42 @@
   </si>
   <si>
     <t>- Identify the backend and the parsing method used.- Assess injection points and try bypassing input filters using HPP.</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/</t>
+  </si>
+  <si>
+    <t>POST http://192.168.1.4:3000/api/Addresss/</t>
+  </si>
+  <si>
+    <t>POST http://192.168.1.4:3000/api/BasketItems/</t>
+  </si>
+  <si>
+    <t>POST http://192.168.1.4:3000/api/Cards/</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Challenges/?name=&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Deliverys/&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/api/Products/?d=&lt;value&gt;</t>
+  </si>
+  <si>
+    <t>POST http://192.168.1.4:3000/api/SecurityAnswers/</t>
+  </si>
+  <si>
+    <t>POST http://192.168.1.4:3000/api/Users/</t>
+  </si>
+  <si>
+    <t>POST http://192.168.1.4:3000/rest/user/login</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/rest/wallet/balance</t>
+  </si>
+  <si>
+    <t>GET http://192.168.1.4:3000/socket.io/?EIO=&lt;value&gt;&amp;transport=&lt;value&gt;&amp;t=&lt;value&gt;&amp;sid=&lt;value&gt;</t>
   </si>
   <si>
     <t>WSTG-INPV-05</t>
@@ -1493,7 +1565,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G131"/>
+  <dimension ref="A1:G160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
@@ -1567,7 +1639,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="100" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -1582,7 +1654,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="100" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1597,7 +1669,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="100" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1612,7 +1684,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="100" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -1627,7 +1699,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="100" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
@@ -1642,7 +1714,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="100" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
@@ -1657,7 +1729,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="100" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
@@ -1672,7 +1744,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="100" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
@@ -1687,7 +1759,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="100" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>39</v>
       </c>
@@ -1702,7 +1774,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" ht="100" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -1717,6 +1789,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
+    <row r="17" spans="1:7" ht="100" customHeight="1"/>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
         <v>45</v>
@@ -1740,7 +1813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="100" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>46</v>
       </c>
@@ -1755,7 +1828,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" ht="100" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>49</v>
       </c>
@@ -1770,7 +1843,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="100" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>52</v>
       </c>
@@ -1785,7 +1858,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="100" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>55</v>
       </c>
@@ -1800,7 +1873,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="100" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>58</v>
       </c>
@@ -1815,7 +1888,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="100" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>61</v>
       </c>
@@ -1830,7 +1903,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="100" customHeight="1">
       <c r="A25" s="5" t="s">
         <v>64</v>
       </c>
@@ -1845,7 +1918,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="100" customHeight="1">
       <c r="A26" s="5" t="s">
         <v>67</v>
       </c>
@@ -1860,7 +1933,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" ht="100" customHeight="1">
       <c r="A27" s="5" t="s">
         <v>69</v>
       </c>
@@ -1875,7 +1948,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" ht="100" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>72</v>
       </c>
@@ -1890,7 +1963,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" ht="100" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>75</v>
       </c>
@@ -1905,7 +1978,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" ht="100" customHeight="1">
       <c r="A30" s="5" t="s">
         <v>78</v>
       </c>
@@ -1920,7 +1993,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" ht="100" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>81</v>
       </c>
@@ -1935,6 +2008,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
+    <row r="32" spans="1:7" ht="100" customHeight="1"/>
     <row r="33" spans="1:7">
       <c r="A33" s="6" t="s">
         <v>84</v>
@@ -1958,7 +2032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" ht="100" customHeight="1">
       <c r="A34" s="4" t="s">
         <v>85</v>
       </c>
@@ -1973,7 +2047,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" ht="100" customHeight="1">
       <c r="A35" s="5" t="s">
         <v>88</v>
       </c>
@@ -1988,7 +2062,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" ht="100" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>91</v>
       </c>
@@ -2003,7 +2077,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" ht="100" customHeight="1">
       <c r="A37" s="5" t="s">
         <v>94</v>
       </c>
@@ -2018,7 +2092,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" ht="100" customHeight="1">
       <c r="A38" s="5" t="s">
         <v>97</v>
       </c>
@@ -2033,6 +2107,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
     </row>
+    <row r="39" spans="1:7" ht="100" customHeight="1"/>
     <row r="40" spans="1:7">
       <c r="A40" s="6" t="s">
         <v>100</v>
@@ -2056,7 +2131,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" ht="100" customHeight="1">
       <c r="A41" s="5" t="s">
         <v>101</v>
       </c>
@@ -2071,7 +2146,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" ht="100" customHeight="1">
       <c r="A42" s="5" t="s">
         <v>103</v>
       </c>
@@ -2086,7 +2161,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" ht="100" customHeight="1">
       <c r="A43" s="5" t="s">
         <v>106</v>
       </c>
@@ -2101,7 +2176,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" ht="100" customHeight="1">
       <c r="A44" s="3" t="s">
         <v>109</v>
       </c>
@@ -2116,7 +2191,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" ht="100" customHeight="1">
       <c r="A45" s="5" t="s">
         <v>112</v>
       </c>
@@ -2131,7 +2206,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" ht="100" customHeight="1">
       <c r="A46" s="5" t="s">
         <v>115</v>
       </c>
@@ -2146,7 +2221,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" ht="100" customHeight="1">
       <c r="A47" s="5" t="s">
         <v>118</v>
       </c>
@@ -2161,7 +2236,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" ht="100" customHeight="1">
       <c r="A48" s="5" t="s">
         <v>121</v>
       </c>
@@ -2176,7 +2251,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" ht="100" customHeight="1">
       <c r="A49" s="3" t="s">
         <v>124</v>
       </c>
@@ -2191,7 +2266,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" ht="100" customHeight="1">
       <c r="A50" s="5" t="s">
         <v>127</v>
       </c>
@@ -2206,6 +2281,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
     </row>
+    <row r="51" spans="1:7" ht="100" customHeight="1"/>
     <row r="52" spans="1:7">
       <c r="A52" s="6" t="s">
         <v>130</v>
@@ -2229,7 +2305,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" ht="100" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>131</v>
       </c>
@@ -2244,7 +2320,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" ht="100" customHeight="1">
       <c r="A54" s="4" t="s">
         <v>134</v>
       </c>
@@ -2259,212 +2335,178 @@
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" ht="100" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="5" t="s">
-        <v>143</v>
+    <row r="56" spans="1:7" ht="100" customHeight="1">
+      <c r="A56" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D56" s="7"/>
+        <v>154</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
     </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="4"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+    </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A58" s="4"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D59" s="7"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D60" s="7"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D61" s="7"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7" t="s">
+        <v>145</v>
+      </c>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D62" s="7"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="D63" s="7"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7" t="s">
+        <v>147</v>
+      </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D64" s="7"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7" t="s">
+        <v>148</v>
+      </c>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D65" s="7"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D66" s="7"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7" t="s">
+        <v>150</v>
+      </c>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D67" s="7"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7" t="s">
+        <v>151</v>
+      </c>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="4" t="s">
-        <v>174</v>
+      <c r="A68" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
     </row>
+    <row r="69" spans="1:7" ht="100" customHeight="1"/>
     <row r="70" spans="1:7">
       <c r="A70" s="6" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>10</v>
@@ -2485,851 +2527,804 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" ht="100" customHeight="1">
       <c r="A71" s="5" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
     </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="4" t="s">
-        <v>181</v>
+    <row r="72" spans="1:7" ht="100" customHeight="1">
+      <c r="A72" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" ht="100" customHeight="1">
       <c r="A73" s="5" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
     </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="3" t="s">
-        <v>189</v>
+    <row r="74" spans="1:7" ht="100" customHeight="1">
+      <c r="A74" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
     </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="3" t="s">
-        <v>192</v>
+    <row r="75" spans="1:7" ht="100" customHeight="1">
+      <c r="A75" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
     </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="4" t="s">
-        <v>195</v>
+    <row r="76" spans="1:7" ht="100" customHeight="1">
+      <c r="A76" s="5" t="s">
+        <v>174</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
     </row>
-    <row r="77" spans="1:7">
-      <c r="A77" s="3" t="s">
-        <v>198</v>
+    <row r="77" spans="1:7" ht="100" customHeight="1">
+      <c r="A77" s="5" t="s">
+        <v>177</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
     </row>
-    <row r="78" spans="1:7">
-      <c r="A78" s="4" t="s">
-        <v>201</v>
+    <row r="78" spans="1:7" ht="100" customHeight="1">
+      <c r="A78" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" ht="100" customHeight="1">
       <c r="A79" s="5" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
     </row>
-    <row r="80" spans="1:7">
-      <c r="A80" s="3" t="s">
-        <v>207</v>
+    <row r="80" spans="1:7" ht="100" customHeight="1">
+      <c r="A80" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
     </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7"/>
-    </row>
+    <row r="81" spans="1:7" ht="100" customHeight="1"/>
     <row r="82" spans="1:7">
-      <c r="A82" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="A83" s="4" t="s">
-        <v>215</v>
+      <c r="A82" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="100" customHeight="1">
+      <c r="A83" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" ht="100" customHeight="1">
       <c r="A84" s="4" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
     </row>
-    <row r="85" spans="1:7">
-      <c r="A85" s="4" t="s">
-        <v>221</v>
+    <row r="85" spans="1:7" ht="100" customHeight="1">
+      <c r="A85" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>223</v>
+        <v>41</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" ht="100" customHeight="1">
       <c r="A86" s="5" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
     </row>
-    <row r="87" spans="1:7">
-      <c r="A87" s="4" t="s">
-        <v>227</v>
+    <row r="87" spans="1:7" ht="100" customHeight="1">
+      <c r="A87" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D87" s="7"/>
+        <v>215</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>201</v>
+      </c>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
     </row>
     <row r="88" spans="1:7">
-      <c r="A88" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D88" s="7"/>
+      <c r="A88" s="3"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7" t="s">
+        <v>202</v>
+      </c>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D89" s="7"/>
+      <c r="A89" s="3"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7" t="s">
+        <v>203</v>
+      </c>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D90" s="7"/>
+      <c r="A90" s="3"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7" t="s">
+        <v>204</v>
+      </c>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
     </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="3"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="7"/>
+    </row>
     <row r="92" spans="1:7">
-      <c r="A92" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F92" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G92" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A92" s="3"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
     </row>
     <row r="93" spans="1:7">
-      <c r="A93" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="D93" s="7"/>
+      <c r="A93" s="3"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7" t="s">
+        <v>207</v>
+      </c>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
     </row>
     <row r="94" spans="1:7">
-      <c r="A94" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D94" s="7"/>
+      <c r="A94" s="3"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7" t="s">
+        <v>208</v>
+      </c>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
     </row>
+    <row r="95" spans="1:7">
+      <c r="A95" s="3"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7"/>
+      <c r="G95" s="7"/>
+    </row>
     <row r="96" spans="1:7">
-      <c r="A96" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E96" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F96" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G96" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A96" s="3"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E96" s="7"/>
+      <c r="F96" s="7"/>
+      <c r="G96" s="7"/>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="D97" s="7"/>
+      <c r="A97" s="3"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7" t="s">
+        <v>148</v>
+      </c>
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
     </row>
     <row r="98" spans="1:7">
-      <c r="A98" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="D98" s="7"/>
+      <c r="A98" s="3"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
     </row>
     <row r="99" spans="1:7">
-      <c r="A99" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="D99" s="7"/>
+      <c r="A99" s="3"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7" t="s">
+        <v>150</v>
+      </c>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
     </row>
     <row r="100" spans="1:7">
-      <c r="A100" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="D100" s="7"/>
+      <c r="A100" s="3"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7" t="s">
+        <v>210</v>
+      </c>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="3"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7"/>
+    </row>
     <row r="102" spans="1:7">
-      <c r="A102" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E102" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F102" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G102" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A102" s="3"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
     </row>
     <row r="103" spans="1:7">
-      <c r="A103" s="4" t="s">
-        <v>259</v>
+      <c r="A103" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>261</v>
+        <v>218</v>
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
     </row>
-    <row r="104" spans="1:7">
-      <c r="A104" s="5" t="s">
-        <v>262</v>
+    <row r="104" spans="1:7" ht="100" customHeight="1">
+      <c r="A104" s="4" t="s">
+        <v>219</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>263</v>
+        <v>220</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>264</v>
+        <v>221</v>
       </c>
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" spans="1:7">
-      <c r="A105" s="5" t="s">
-        <v>265</v>
+    <row r="105" spans="1:7" ht="100" customHeight="1">
+      <c r="A105" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>267</v>
+        <v>224</v>
       </c>
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
     </row>
-    <row r="106" spans="1:7">
-      <c r="A106" s="5" t="s">
-        <v>268</v>
+    <row r="106" spans="1:7" ht="100" customHeight="1">
+      <c r="A106" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>270</v>
+        <v>227</v>
       </c>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" ht="100" customHeight="1">
       <c r="A107" s="5" t="s">
-        <v>271</v>
+        <v>228</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>272</v>
+        <v>229</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>273</v>
+        <v>230</v>
       </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
       <c r="F107" s="7"/>
       <c r="G107" s="7"/>
     </row>
-    <row r="108" spans="1:7">
-      <c r="A108" s="5" t="s">
-        <v>274</v>
+    <row r="108" spans="1:7" ht="100" customHeight="1">
+      <c r="A108" s="3" t="s">
+        <v>231</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>276</v>
+        <v>233</v>
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
     </row>
-    <row r="109" spans="1:7">
-      <c r="A109" s="5" t="s">
-        <v>277</v>
+    <row r="109" spans="1:7" ht="100" customHeight="1">
+      <c r="A109" s="3" t="s">
+        <v>234</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>278</v>
+        <v>235</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>279</v>
+        <v>236</v>
       </c>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
     </row>
-    <row r="110" spans="1:7">
-      <c r="A110" s="5" t="s">
-        <v>280</v>
+    <row r="110" spans="1:7" ht="100" customHeight="1">
+      <c r="A110" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>282</v>
+        <v>41</v>
       </c>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" ht="100" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>283</v>
+        <v>239</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>284</v>
+        <v>240</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>285</v>
+        <v>241</v>
       </c>
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" ht="100" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>286</v>
+        <v>242</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>287</v>
+        <v>243</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>288</v>
+        <v>244</v>
       </c>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
     </row>
-    <row r="114" spans="1:7">
-      <c r="A114" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E114" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F114" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G114" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7">
+    <row r="113" spans="1:7" ht="100" customHeight="1">
+      <c r="A113" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7"/>
+      <c r="G113" s="7"/>
+    </row>
+    <row r="114" spans="1:7" ht="100" customHeight="1">
+      <c r="A114" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D114" s="7"/>
+      <c r="E114" s="7"/>
+      <c r="F114" s="7"/>
+      <c r="G114" s="7"/>
+    </row>
+    <row r="115" spans="1:7" ht="100" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>290</v>
+        <v>251</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>291</v>
+        <v>252</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
       <c r="F115" s="7"/>
       <c r="G115" s="7"/>
     </row>
-    <row r="116" spans="1:7">
-      <c r="A116" s="5" t="s">
-        <v>293</v>
+    <row r="116" spans="1:7" ht="100" customHeight="1">
+      <c r="A116" s="3" t="s">
+        <v>254</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>294</v>
+        <v>255</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>295</v>
+        <v>256</v>
       </c>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
     </row>
-    <row r="117" spans="1:7">
-      <c r="A117" s="5" t="s">
-        <v>296</v>
+    <row r="117" spans="1:7" ht="100" customHeight="1">
+      <c r="A117" s="4" t="s">
+        <v>257</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>297</v>
+        <v>258</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>298</v>
+        <v>259</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
       <c r="F117" s="7"/>
       <c r="G117" s="7"/>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" ht="100" customHeight="1">
       <c r="A118" s="5" t="s">
-        <v>299</v>
+        <v>260</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>300</v>
+        <v>261</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>301</v>
+        <v>262</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
       <c r="F118" s="7"/>
       <c r="G118" s="7"/>
     </row>
-    <row r="119" spans="1:7">
-      <c r="A119" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="D119" s="7"/>
-      <c r="E119" s="7"/>
-      <c r="F119" s="7"/>
-      <c r="G119" s="7"/>
-    </row>
+    <row r="119" spans="1:7" ht="100" customHeight="1"/>
     <row r="120" spans="1:7">
-      <c r="A120" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="D120" s="7"/>
-      <c r="E120" s="7"/>
-      <c r="F120" s="7"/>
-      <c r="G120" s="7"/>
-    </row>
-    <row r="121" spans="1:7">
+      <c r="A120" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G120" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="100" customHeight="1">
       <c r="A121" s="5" t="s">
-        <v>308</v>
+        <v>264</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>309</v>
+        <v>265</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>310</v>
+        <v>266</v>
       </c>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" ht="100" customHeight="1">
       <c r="A122" s="5" t="s">
-        <v>311</v>
+        <v>267</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>312</v>
+        <v>268</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>313</v>
+        <v>41</v>
       </c>
       <c r="D122" s="7"/>
       <c r="E122" s="7"/>
       <c r="F122" s="7"/>
       <c r="G122" s="7"/>
     </row>
-    <row r="123" spans="1:7">
-      <c r="A123" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="B123" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C123" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="D123" s="7"/>
-      <c r="E123" s="7"/>
-      <c r="F123" s="7"/>
-      <c r="G123" s="7"/>
-    </row>
+    <row r="123" spans="1:7" ht="100" customHeight="1"/>
     <row r="124" spans="1:7">
-      <c r="A124" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B124" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="D124" s="7"/>
-      <c r="E124" s="7"/>
-      <c r="F124" s="7"/>
-      <c r="G124" s="7"/>
-    </row>
-    <row r="125" spans="1:7">
+      <c r="A124" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G124" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="100" customHeight="1">
       <c r="A125" s="5" t="s">
-        <v>320</v>
+        <v>270</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>321</v>
+        <v>271</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" ht="100" customHeight="1">
       <c r="A126" s="5" t="s">
-        <v>323</v>
+        <v>273</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
       <c r="F126" s="7"/>
       <c r="G126" s="7"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" ht="100" customHeight="1">
       <c r="A127" s="5" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>327</v>
+        <v>277</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
       <c r="D127" s="7"/>
       <c r="E127" s="7"/>
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" ht="100" customHeight="1">
       <c r="A128" s="5" t="s">
-        <v>329</v>
+        <v>279</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>41</v>
+        <v>281</v>
       </c>
       <c r="D128" s="7"/>
       <c r="E128" s="7"/>
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
     </row>
+    <row r="129" spans="1:7" ht="100" customHeight="1"/>
     <row r="130" spans="1:7">
       <c r="A130" s="6" t="s">
-        <v>331</v>
+        <v>282</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>10</v>
@@ -3350,37 +3345,446 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" ht="100" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>332</v>
+        <v>283</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>333</v>
+        <v>284</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>334</v>
+        <v>285</v>
       </c>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
     </row>
+    <row r="132" spans="1:7" ht="100" customHeight="1">
+      <c r="A132" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D132" s="7"/>
+      <c r="E132" s="7"/>
+      <c r="F132" s="7"/>
+      <c r="G132" s="7"/>
+    </row>
+    <row r="133" spans="1:7" ht="100" customHeight="1">
+      <c r="A133" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7"/>
+      <c r="G133" s="7"/>
+    </row>
+    <row r="134" spans="1:7" ht="100" customHeight="1">
+      <c r="A134" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="D134" s="7"/>
+      <c r="E134" s="7"/>
+      <c r="F134" s="7"/>
+      <c r="G134" s="7"/>
+    </row>
+    <row r="135" spans="1:7" ht="100" customHeight="1">
+      <c r="A135" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="D135" s="7"/>
+      <c r="E135" s="7"/>
+      <c r="F135" s="7"/>
+      <c r="G135" s="7"/>
+    </row>
+    <row r="136" spans="1:7" ht="100" customHeight="1">
+      <c r="A136" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D136" s="7"/>
+      <c r="E136" s="7"/>
+      <c r="F136" s="7"/>
+      <c r="G136" s="7"/>
+    </row>
+    <row r="137" spans="1:7" ht="100" customHeight="1">
+      <c r="A137" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="D137" s="7"/>
+      <c r="E137" s="7"/>
+      <c r="F137" s="7"/>
+      <c r="G137" s="7"/>
+    </row>
+    <row r="138" spans="1:7" ht="100" customHeight="1">
+      <c r="A138" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="D138" s="7"/>
+      <c r="E138" s="7"/>
+      <c r="F138" s="7"/>
+      <c r="G138" s="7"/>
+    </row>
+    <row r="139" spans="1:7" ht="100" customHeight="1">
+      <c r="A139" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="D139" s="7"/>
+      <c r="E139" s="7"/>
+      <c r="F139" s="7"/>
+      <c r="G139" s="7"/>
+    </row>
+    <row r="140" spans="1:7" ht="100" customHeight="1">
+      <c r="A140" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="D140" s="7"/>
+      <c r="E140" s="7"/>
+      <c r="F140" s="7"/>
+      <c r="G140" s="7"/>
+    </row>
+    <row r="141" spans="1:7" ht="100" customHeight="1"/>
+    <row r="142" spans="1:7">
+      <c r="A142" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D142" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G142" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="100" customHeight="1">
+      <c r="A143" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D143" s="7"/>
+      <c r="E143" s="7"/>
+      <c r="F143" s="7"/>
+      <c r="G143" s="7"/>
+    </row>
+    <row r="144" spans="1:7" ht="100" customHeight="1">
+      <c r="A144" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="D144" s="7"/>
+      <c r="E144" s="7"/>
+      <c r="F144" s="7"/>
+      <c r="G144" s="7"/>
+    </row>
+    <row r="145" spans="1:7" ht="100" customHeight="1">
+      <c r="A145" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="D145" s="7"/>
+      <c r="E145" s="7"/>
+      <c r="F145" s="7"/>
+      <c r="G145" s="7"/>
+    </row>
+    <row r="146" spans="1:7" ht="100" customHeight="1">
+      <c r="A146" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="C146" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="D146" s="7"/>
+      <c r="E146" s="7"/>
+      <c r="F146" s="7"/>
+      <c r="G146" s="7"/>
+    </row>
+    <row r="147" spans="1:7" ht="100" customHeight="1">
+      <c r="A147" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7"/>
+      <c r="F147" s="7"/>
+      <c r="G147" s="7"/>
+    </row>
+    <row r="148" spans="1:7" ht="100" customHeight="1">
+      <c r="A148" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C148" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D148" s="7"/>
+      <c r="E148" s="7"/>
+      <c r="F148" s="7"/>
+      <c r="G148" s="7"/>
+    </row>
+    <row r="149" spans="1:7" ht="100" customHeight="1">
+      <c r="A149" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+      <c r="F149" s="7"/>
+      <c r="G149" s="7"/>
+    </row>
+    <row r="150" spans="1:7" ht="100" customHeight="1">
+      <c r="A150" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="D150" s="7"/>
+      <c r="E150" s="7"/>
+      <c r="F150" s="7"/>
+      <c r="G150" s="7"/>
+    </row>
+    <row r="151" spans="1:7" ht="100" customHeight="1">
+      <c r="A151" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="D151" s="7"/>
+      <c r="E151" s="7"/>
+      <c r="F151" s="7"/>
+      <c r="G151" s="7"/>
+    </row>
+    <row r="152" spans="1:7" ht="100" customHeight="1">
+      <c r="A152" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="D152" s="7"/>
+      <c r="E152" s="7"/>
+      <c r="F152" s="7"/>
+      <c r="G152" s="7"/>
+    </row>
+    <row r="153" spans="1:7" ht="100" customHeight="1">
+      <c r="A153" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="C153" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D153" s="7"/>
+      <c r="E153" s="7"/>
+      <c r="F153" s="7"/>
+      <c r="G153" s="7"/>
+    </row>
+    <row r="154" spans="1:7" ht="100" customHeight="1">
+      <c r="A154" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="D154" s="7"/>
+      <c r="E154" s="7"/>
+      <c r="F154" s="7"/>
+      <c r="G154" s="7"/>
+    </row>
+    <row r="155" spans="1:7" ht="100" customHeight="1">
+      <c r="A155" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="D155" s="7"/>
+      <c r="E155" s="7"/>
+      <c r="F155" s="7"/>
+      <c r="G155" s="7"/>
+    </row>
+    <row r="156" spans="1:7" ht="100" customHeight="1">
+      <c r="A156" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D156" s="7"/>
+      <c r="E156" s="7"/>
+      <c r="F156" s="7"/>
+      <c r="G156" s="7"/>
+    </row>
+    <row r="157" spans="1:7" ht="100" customHeight="1"/>
+    <row r="158" spans="1:7">
+      <c r="A158" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B158" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E158" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F158" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G158" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="100" customHeight="1">
+      <c r="A159" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7"/>
+      <c r="F159" s="7"/>
+      <c r="G159" s="7"/>
+    </row>
+    <row r="160" spans="1:7" ht="100" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="G74:G75"/>
+    <mergeCell ref="A56:A67"/>
+    <mergeCell ref="B56:B67"/>
+    <mergeCell ref="C56:C67"/>
+    <mergeCell ref="F56:F67"/>
+    <mergeCell ref="G56:G67"/>
+    <mergeCell ref="A87:A102"/>
+    <mergeCell ref="B87:B102"/>
+    <mergeCell ref="C87:C102"/>
+    <mergeCell ref="F87:F102"/>
+    <mergeCell ref="G87:G102"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7:E131">
+  <conditionalFormatting sqref="E7:E159">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"VULN"</formula>
     </cfRule>
@@ -3389,7 +3793,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E159">
       <formula1>"PASSED,VULN"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
feat: update filter on mapper
</commit_message>
<xml_diff>
--- a/report/coba.xlsx
+++ b/report/coba.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="360">
   <si>
     <t>OWASP: Testing Guide v4.2 Checklist</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>- Identify what sensitive design and configuration information of the application, system, or organization is exposed directly (on the organization's site) or indirectly (via third-party services).</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
   <si>
     <t>WSTG-INFO-02</t>
@@ -1649,142 +1652,162 @@
       <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="100" customHeight="1">
       <c r="A8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="100" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="100" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="100" customHeight="1">
       <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="100" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" ht="100" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="100" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="100" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="100" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -1792,7 +1815,7 @@
     <row r="17" spans="1:7" ht="100" customHeight="1"/>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>10</v>
@@ -1815,195 +1838,221 @@
     </row>
     <row r="19" spans="1:7" ht="100" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="7"/>
+        <v>49</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="100" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" ht="100" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="7"/>
+        <v>55</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" ht="100" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" ht="100" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="7"/>
+        <v>61</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" ht="100" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="7"/>
+        <v>64</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" ht="100" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" ht="100" customHeight="1">
       <c r="A26" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" ht="100" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" ht="100" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" ht="100" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="7"/>
+        <v>78</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" ht="100" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" ht="100" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="7"/>
+        <v>84</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -2011,7 +2060,7 @@
     <row r="32" spans="1:7" ht="100" customHeight="1"/>
     <row r="33" spans="1:7">
       <c r="A33" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>10</v>
@@ -2034,13 +2083,13 @@
     </row>
     <row r="34" spans="1:7" ht="100" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -2049,13 +2098,13 @@
     </row>
     <row r="35" spans="1:7" ht="100" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -2064,13 +2113,13 @@
     </row>
     <row r="36" spans="1:7" ht="100" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -2079,13 +2128,13 @@
     </row>
     <row r="37" spans="1:7" ht="100" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -2094,13 +2143,13 @@
     </row>
     <row r="38" spans="1:7" ht="100" customHeight="1">
       <c r="A38" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -2110,7 +2159,7 @@
     <row r="39" spans="1:7" ht="100" customHeight="1"/>
     <row r="40" spans="1:7">
       <c r="A40" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>10</v>
@@ -2133,13 +2182,13 @@
     </row>
     <row r="41" spans="1:7" ht="100" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
@@ -2148,13 +2197,13 @@
     </row>
     <row r="42" spans="1:7" ht="100" customHeight="1">
       <c r="A42" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
@@ -2163,13 +2212,13 @@
     </row>
     <row r="43" spans="1:7" ht="100" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -2178,13 +2227,13 @@
     </row>
     <row r="44" spans="1:7" ht="100" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -2193,13 +2242,13 @@
     </row>
     <row r="45" spans="1:7" ht="100" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -2208,13 +2257,13 @@
     </row>
     <row r="46" spans="1:7" ht="100" customHeight="1">
       <c r="A46" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -2223,13 +2272,13 @@
     </row>
     <row r="47" spans="1:7" ht="100" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -2238,13 +2287,13 @@
     </row>
     <row r="48" spans="1:7" ht="100" customHeight="1">
       <c r="A48" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -2253,13 +2302,13 @@
     </row>
     <row r="49" spans="1:7" ht="100" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -2268,13 +2317,13 @@
     </row>
     <row r="50" spans="1:7" ht="100" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
@@ -2284,7 +2333,7 @@
     <row r="51" spans="1:7" ht="100" customHeight="1"/>
     <row r="52" spans="1:7">
       <c r="A52" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>10</v>
@@ -2307,13 +2356,13 @@
     </row>
     <row r="53" spans="1:7" ht="100" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
@@ -2322,13 +2371,13 @@
     </row>
     <row r="54" spans="1:7" ht="100" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
@@ -2337,13 +2386,13 @@
     </row>
     <row r="55" spans="1:7" ht="100" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -2352,16 +2401,16 @@
     </row>
     <row r="56" spans="1:7" ht="100" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
@@ -2372,7 +2421,7 @@
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
@@ -2383,7 +2432,7 @@
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
@@ -2394,7 +2443,7 @@
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
@@ -2405,7 +2454,7 @@
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
@@ -2416,7 +2465,7 @@
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
@@ -2427,7 +2476,7 @@
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
@@ -2438,7 +2487,7 @@
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
@@ -2449,7 +2498,7 @@
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
@@ -2460,7 +2509,7 @@
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
@@ -2471,7 +2520,7 @@
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
@@ -2482,7 +2531,7 @@
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
@@ -2490,13 +2539,13 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
@@ -2506,7 +2555,7 @@
     <row r="69" spans="1:7" ht="100" customHeight="1"/>
     <row r="70" spans="1:7">
       <c r="A70" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>10</v>
@@ -2529,13 +2578,13 @@
     </row>
     <row r="71" spans="1:7" ht="100" customHeight="1">
       <c r="A71" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
@@ -2544,13 +2593,13 @@
     </row>
     <row r="72" spans="1:7" ht="100" customHeight="1">
       <c r="A72" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
@@ -2559,13 +2608,13 @@
     </row>
     <row r="73" spans="1:7" ht="100" customHeight="1">
       <c r="A73" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
@@ -2574,13 +2623,13 @@
     </row>
     <row r="74" spans="1:7" ht="100" customHeight="1">
       <c r="A74" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
@@ -2589,13 +2638,13 @@
     </row>
     <row r="75" spans="1:7" ht="100" customHeight="1">
       <c r="A75" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
@@ -2604,13 +2653,13 @@
     </row>
     <row r="76" spans="1:7" ht="100" customHeight="1">
       <c r="A76" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
@@ -2619,13 +2668,13 @@
     </row>
     <row r="77" spans="1:7" ht="100" customHeight="1">
       <c r="A77" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
@@ -2634,13 +2683,13 @@
     </row>
     <row r="78" spans="1:7" ht="100" customHeight="1">
       <c r="A78" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
@@ -2649,13 +2698,13 @@
     </row>
     <row r="79" spans="1:7" ht="100" customHeight="1">
       <c r="A79" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
@@ -2664,13 +2713,13 @@
     </row>
     <row r="80" spans="1:7" ht="100" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
@@ -2680,7 +2729,7 @@
     <row r="81" spans="1:7" ht="100" customHeight="1"/>
     <row r="82" spans="1:7">
       <c r="A82" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>10</v>
@@ -2703,13 +2752,13 @@
     </row>
     <row r="83" spans="1:7" ht="100" customHeight="1">
       <c r="A83" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
@@ -2718,13 +2767,13 @@
     </row>
     <row r="84" spans="1:7" ht="100" customHeight="1">
       <c r="A84" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
@@ -2733,13 +2782,13 @@
     </row>
     <row r="85" spans="1:7" ht="100" customHeight="1">
       <c r="A85" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
@@ -2748,13 +2797,13 @@
     </row>
     <row r="86" spans="1:7" ht="100" customHeight="1">
       <c r="A86" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
@@ -2763,16 +2812,16 @@
     </row>
     <row r="87" spans="1:7" ht="100" customHeight="1">
       <c r="A87" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
@@ -2783,7 +2832,7 @@
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
@@ -2794,7 +2843,7 @@
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
@@ -2805,7 +2854,7 @@
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
@@ -2816,7 +2865,7 @@
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
@@ -2827,7 +2876,7 @@
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E92" s="7"/>
       <c r="F92" s="7"/>
@@ -2838,7 +2887,7 @@
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
@@ -2849,7 +2898,7 @@
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
@@ -2860,7 +2909,7 @@
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
@@ -2871,7 +2920,7 @@
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
@@ -2882,7 +2931,7 @@
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
@@ -2893,7 +2942,7 @@
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
@@ -2904,7 +2953,7 @@
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
@@ -2915,7 +2964,7 @@
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
@@ -2926,7 +2975,7 @@
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
@@ -2937,7 +2986,7 @@
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
@@ -2945,13 +2994,13 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
@@ -2960,13 +3009,13 @@
     </row>
     <row r="104" spans="1:7" ht="100" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
@@ -2975,13 +3024,13 @@
     </row>
     <row r="105" spans="1:7" ht="100" customHeight="1">
       <c r="A105" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
@@ -2990,13 +3039,13 @@
     </row>
     <row r="106" spans="1:7" ht="100" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
@@ -3005,13 +3054,13 @@
     </row>
     <row r="107" spans="1:7" ht="100" customHeight="1">
       <c r="A107" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
@@ -3020,13 +3069,13 @@
     </row>
     <row r="108" spans="1:7" ht="100" customHeight="1">
       <c r="A108" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
@@ -3035,13 +3084,13 @@
     </row>
     <row r="109" spans="1:7" ht="100" customHeight="1">
       <c r="A109" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
@@ -3050,13 +3099,13 @@
     </row>
     <row r="110" spans="1:7" ht="100" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
@@ -3065,13 +3114,13 @@
     </row>
     <row r="111" spans="1:7" ht="100" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
@@ -3080,13 +3129,13 @@
     </row>
     <row r="112" spans="1:7" ht="100" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
@@ -3095,13 +3144,13 @@
     </row>
     <row r="113" spans="1:7" ht="100" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
@@ -3110,13 +3159,13 @@
     </row>
     <row r="114" spans="1:7" ht="100" customHeight="1">
       <c r="A114" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
@@ -3125,13 +3174,13 @@
     </row>
     <row r="115" spans="1:7" ht="100" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
@@ -3140,13 +3189,13 @@
     </row>
     <row r="116" spans="1:7" ht="100" customHeight="1">
       <c r="A116" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
@@ -3155,13 +3204,13 @@
     </row>
     <row r="117" spans="1:7" ht="100" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
@@ -3170,13 +3219,13 @@
     </row>
     <row r="118" spans="1:7" ht="100" customHeight="1">
       <c r="A118" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
@@ -3186,7 +3235,7 @@
     <row r="119" spans="1:7" ht="100" customHeight="1"/>
     <row r="120" spans="1:7">
       <c r="A120" s="6" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>10</v>
@@ -3209,13 +3258,13 @@
     </row>
     <row r="121" spans="1:7" ht="100" customHeight="1">
       <c r="A121" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
@@ -3224,13 +3273,13 @@
     </row>
     <row r="122" spans="1:7" ht="100" customHeight="1">
       <c r="A122" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D122" s="7"/>
       <c r="E122" s="7"/>
@@ -3240,7 +3289,7 @@
     <row r="123" spans="1:7" ht="100" customHeight="1"/>
     <row r="124" spans="1:7">
       <c r="A124" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>10</v>
@@ -3263,13 +3312,13 @@
     </row>
     <row r="125" spans="1:7" ht="100" customHeight="1">
       <c r="A125" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
@@ -3278,13 +3327,13 @@
     </row>
     <row r="126" spans="1:7" ht="100" customHeight="1">
       <c r="A126" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
@@ -3293,13 +3342,13 @@
     </row>
     <row r="127" spans="1:7" ht="100" customHeight="1">
       <c r="A127" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D127" s="7"/>
       <c r="E127" s="7"/>
@@ -3308,13 +3357,13 @@
     </row>
     <row r="128" spans="1:7" ht="100" customHeight="1">
       <c r="A128" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D128" s="7"/>
       <c r="E128" s="7"/>
@@ -3324,7 +3373,7 @@
     <row r="129" spans="1:7" ht="100" customHeight="1"/>
     <row r="130" spans="1:7">
       <c r="A130" s="6" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>10</v>
@@ -3347,13 +3396,13 @@
     </row>
     <row r="131" spans="1:7" ht="100" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
@@ -3362,13 +3411,13 @@
     </row>
     <row r="132" spans="1:7" ht="100" customHeight="1">
       <c r="A132" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D132" s="7"/>
       <c r="E132" s="7"/>
@@ -3377,13 +3426,13 @@
     </row>
     <row r="133" spans="1:7" ht="100" customHeight="1">
       <c r="A133" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>
@@ -3392,13 +3441,13 @@
     </row>
     <row r="134" spans="1:7" ht="100" customHeight="1">
       <c r="A134" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="7"/>
@@ -3407,13 +3456,13 @@
     </row>
     <row r="135" spans="1:7" ht="100" customHeight="1">
       <c r="A135" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="7"/>
@@ -3422,13 +3471,13 @@
     </row>
     <row r="136" spans="1:7" ht="100" customHeight="1">
       <c r="A136" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D136" s="7"/>
       <c r="E136" s="7"/>
@@ -3437,13 +3486,13 @@
     </row>
     <row r="137" spans="1:7" ht="100" customHeight="1">
       <c r="A137" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D137" s="7"/>
       <c r="E137" s="7"/>
@@ -3452,13 +3501,13 @@
     </row>
     <row r="138" spans="1:7" ht="100" customHeight="1">
       <c r="A138" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D138" s="7"/>
       <c r="E138" s="7"/>
@@ -3467,13 +3516,13 @@
     </row>
     <row r="139" spans="1:7" ht="100" customHeight="1">
       <c r="A139" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
@@ -3482,13 +3531,13 @@
     </row>
     <row r="140" spans="1:7" ht="100" customHeight="1">
       <c r="A140" s="4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D140" s="7"/>
       <c r="E140" s="7"/>
@@ -3498,7 +3547,7 @@
     <row r="141" spans="1:7" ht="100" customHeight="1"/>
     <row r="142" spans="1:7">
       <c r="A142" s="6" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>10</v>
@@ -3521,13 +3570,13 @@
     </row>
     <row r="143" spans="1:7" ht="100" customHeight="1">
       <c r="A143" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D143" s="7"/>
       <c r="E143" s="7"/>
@@ -3536,13 +3585,13 @@
     </row>
     <row r="144" spans="1:7" ht="100" customHeight="1">
       <c r="A144" s="5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D144" s="7"/>
       <c r="E144" s="7"/>
@@ -3551,13 +3600,13 @@
     </row>
     <row r="145" spans="1:7" ht="100" customHeight="1">
       <c r="A145" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D145" s="7"/>
       <c r="E145" s="7"/>
@@ -3566,13 +3615,13 @@
     </row>
     <row r="146" spans="1:7" ht="100" customHeight="1">
       <c r="A146" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D146" s="7"/>
       <c r="E146" s="7"/>
@@ -3581,13 +3630,13 @@
     </row>
     <row r="147" spans="1:7" ht="100" customHeight="1">
       <c r="A147" s="5" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D147" s="7"/>
       <c r="E147" s="7"/>
@@ -3596,13 +3645,13 @@
     </row>
     <row r="148" spans="1:7" ht="100" customHeight="1">
       <c r="A148" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D148" s="7"/>
       <c r="E148" s="7"/>
@@ -3611,13 +3660,13 @@
     </row>
     <row r="149" spans="1:7" ht="100" customHeight="1">
       <c r="A149" s="5" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D149" s="7"/>
       <c r="E149" s="7"/>
@@ -3626,13 +3675,13 @@
     </row>
     <row r="150" spans="1:7" ht="100" customHeight="1">
       <c r="A150" s="5" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D150" s="7"/>
       <c r="E150" s="7"/>
@@ -3641,13 +3690,13 @@
     </row>
     <row r="151" spans="1:7" ht="100" customHeight="1">
       <c r="A151" s="5" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D151" s="7"/>
       <c r="E151" s="7"/>
@@ -3656,13 +3705,13 @@
     </row>
     <row r="152" spans="1:7" ht="100" customHeight="1">
       <c r="A152" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
@@ -3671,13 +3720,13 @@
     </row>
     <row r="153" spans="1:7" ht="100" customHeight="1">
       <c r="A153" s="5" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
@@ -3686,13 +3735,13 @@
     </row>
     <row r="154" spans="1:7" ht="100" customHeight="1">
       <c r="A154" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
@@ -3701,13 +3750,13 @@
     </row>
     <row r="155" spans="1:7" ht="100" customHeight="1">
       <c r="A155" s="5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
@@ -3716,13 +3765,13 @@
     </row>
     <row r="156" spans="1:7" ht="100" customHeight="1">
       <c r="A156" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D156" s="7"/>
       <c r="E156" s="7"/>
@@ -3732,7 +3781,7 @@
     <row r="157" spans="1:7" ht="100" customHeight="1"/>
     <row r="158" spans="1:7">
       <c r="A158" s="6" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B158" s="6" t="s">
         <v>10</v>
@@ -3755,13 +3804,13 @@
     </row>
     <row r="159" spans="1:7" ht="100" customHeight="1">
       <c r="A159" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D159" s="7"/>
       <c r="E159" s="7"/>

</xml_diff>

<commit_message>
feat: patch assign simple
</commit_message>
<xml_diff>
--- a/report/coba.xlsx
+++ b/report/coba.xlsx
@@ -14,18 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="335">
   <si>
     <t>OWASP: Testing Guide v4.2 Checklist</t>
   </si>
   <si>
-    <t>Target URL/IP : 192.168.1.14:8080</t>
+    <t>Target URL/IP : 192.168.1.14:3000</t>
   </si>
   <si>
     <t xml:space="preserve">Target Name : </t>
   </si>
   <si>
-    <t>Start Date : 2023-06-10</t>
+    <t>Start Date : 2023-06-12</t>
   </si>
   <si>
     <t xml:space="preserve">Pentester Name : </t>
@@ -73,9 +73,6 @@
     <t>- Identify what sensitive design and configuration information of the application, system, or organization is exposed directly (on the organization's site) or indirectly (via third-party services).</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>WSTG-INFO-02</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
     <t>- Verify that the identity requirements for user registration are aligned with business and security requirements.- Validate the registration process.</t>
   </si>
   <si>
-    <t>POST http://192.168.1.14:8080/</t>
-  </si>
-  <si>
     <t>WSTG-IDNT-03</t>
   </si>
   <si>
@@ -479,9 +473,6 @@
   </si>
   <si>
     <t>- Ensure that the proper security configuration is set for cookies.</t>
-  </si>
-  <si>
-    <t>GET http://192.168.1.14:8080/</t>
   </si>
   <si>
     <t>WSTG-SESS-03</t>
@@ -1613,162 +1604,142 @@
       <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="100" customHeight="1">
       <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="100" customHeight="1">
       <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="100" customHeight="1">
       <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="100" customHeight="1">
       <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="100" customHeight="1">
       <c r="A12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" ht="100" customHeight="1">
       <c r="A13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="100" customHeight="1">
       <c r="A14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="100" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="100" customHeight="1">
       <c r="A16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -1776,7 +1747,7 @@
     <row r="17" spans="1:7" ht="100" customHeight="1"/>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>10</v>
@@ -1799,221 +1770,195 @@
     </row>
     <row r="19" spans="1:7" ht="100" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="100" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" ht="100" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" ht="100" customHeight="1">
       <c r="A22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" ht="100" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" ht="100" customHeight="1">
       <c r="A24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" ht="100" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" ht="100" customHeight="1">
       <c r="A26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="C26" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" ht="100" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" ht="100" customHeight="1">
       <c r="A28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" ht="100" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" ht="100" customHeight="1">
       <c r="A30" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" ht="100" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -2021,7 +1966,7 @@
     <row r="32" spans="1:7" ht="100" customHeight="1"/>
     <row r="33" spans="1:7">
       <c r="A33" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>10</v>
@@ -2044,13 +1989,13 @@
     </row>
     <row r="34" spans="1:7" ht="100" customHeight="1">
       <c r="A34" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -2059,64 +2004,58 @@
     </row>
     <row r="35" spans="1:7" ht="100" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>92</v>
-      </c>
+      <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" ht="100" customHeight="1">
       <c r="A36" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>92</v>
-      </c>
+      <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" ht="100" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>92</v>
-      </c>
+      <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" ht="100" customHeight="1">
       <c r="A38" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -2126,7 +2065,7 @@
     <row r="39" spans="1:7" ht="100" customHeight="1"/>
     <row r="40" spans="1:7">
       <c r="A40" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>10</v>
@@ -2149,64 +2088,58 @@
     </row>
     <row r="41" spans="1:7" ht="100" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:7" ht="100" customHeight="1">
       <c r="A42" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>92</v>
-      </c>
+      <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:7" ht="100" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>92</v>
-      </c>
+      <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:7" ht="100" customHeight="1">
       <c r="A44" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -2215,13 +2148,13 @@
     </row>
     <row r="45" spans="1:7" ht="100" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>116</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -2230,13 +2163,13 @@
     </row>
     <row r="46" spans="1:7" ht="100" customHeight="1">
       <c r="A46" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -2245,30 +2178,28 @@
     </row>
     <row r="47" spans="1:7" ht="100" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>92</v>
-      </c>
+      <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" ht="100" customHeight="1">
       <c r="A48" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -2277,34 +2208,30 @@
     </row>
     <row r="49" spans="1:7" ht="100" customHeight="1">
       <c r="A49" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>92</v>
-      </c>
+      <c r="D49" s="7"/>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:7" ht="100" customHeight="1">
       <c r="A50" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
@@ -2312,7 +2239,7 @@
     <row r="51" spans="1:7" ht="100" customHeight="1"/>
     <row r="52" spans="1:7">
       <c r="A52" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>10</v>
@@ -2335,13 +2262,13 @@
     </row>
     <row r="53" spans="1:7" ht="100" customHeight="1">
       <c r="A53" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>135</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
@@ -2350,13 +2277,13 @@
     </row>
     <row r="54" spans="1:7" ht="100" customHeight="1">
       <c r="A54" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
@@ -2365,13 +2292,13 @@
     </row>
     <row r="55" spans="1:7" ht="100" customHeight="1">
       <c r="A55" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -2380,13 +2307,13 @@
     </row>
     <row r="56" spans="1:7" ht="100" customHeight="1">
       <c r="A56" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>144</v>
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
@@ -2395,13 +2322,13 @@
     </row>
     <row r="57" spans="1:7" ht="100" customHeight="1">
       <c r="A57" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
@@ -2411,7 +2338,7 @@
     <row r="58" spans="1:7" ht="100" customHeight="1"/>
     <row r="59" spans="1:7">
       <c r="A59" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>10</v>
@@ -2434,13 +2361,13 @@
     </row>
     <row r="60" spans="1:7" ht="100" customHeight="1">
       <c r="A60" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>151</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
@@ -2449,81 +2376,73 @@
     </row>
     <row r="61" spans="1:7" ht="100" customHeight="1">
       <c r="A61" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B61" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>155</v>
-      </c>
+      <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
     </row>
     <row r="62" spans="1:7" ht="100" customHeight="1">
       <c r="A62" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D62" s="7" t="s">
         <v>155</v>
       </c>
+      <c r="D62" s="7"/>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
     </row>
     <row r="63" spans="1:7" ht="100" customHeight="1">
       <c r="A63" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>155</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="D63" s="7"/>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
     </row>
     <row r="64" spans="1:7" ht="100" customHeight="1">
       <c r="A64" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>155</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
     </row>
     <row r="65" spans="1:7" ht="100" customHeight="1">
       <c r="A65" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
@@ -2532,13 +2451,13 @@
     </row>
     <row r="66" spans="1:7" ht="100" customHeight="1">
       <c r="A66" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
@@ -2547,13 +2466,13 @@
     </row>
     <row r="67" spans="1:7" ht="100" customHeight="1">
       <c r="A67" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
@@ -2562,30 +2481,28 @@
     </row>
     <row r="68" spans="1:7" ht="100" customHeight="1">
       <c r="A68" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
     </row>
     <row r="69" spans="1:7" ht="100" customHeight="1">
       <c r="A69" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
@@ -2595,7 +2512,7 @@
     <row r="70" spans="1:7" ht="100" customHeight="1"/>
     <row r="71" spans="1:7">
       <c r="A71" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>10</v>
@@ -2618,115 +2535,103 @@
     </row>
     <row r="72" spans="1:7" ht="100" customHeight="1">
       <c r="A72" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="D72" s="7"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
     </row>
     <row r="73" spans="1:7" ht="100" customHeight="1">
       <c r="A73" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="D73" s="7"/>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
     </row>
     <row r="74" spans="1:7" ht="100" customHeight="1">
       <c r="A74" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D74" s="7"/>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
     </row>
     <row r="75" spans="1:7" ht="100" customHeight="1">
       <c r="A75" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="D75" s="7"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
     </row>
     <row r="76" spans="1:7" ht="100" customHeight="1">
       <c r="A76" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
     </row>
     <row r="77" spans="1:7" ht="100" customHeight="1">
       <c r="A77" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="D77" s="7"/>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
     </row>
     <row r="78" spans="1:7" ht="100" customHeight="1">
       <c r="A78" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
@@ -2735,13 +2640,13 @@
     </row>
     <row r="79" spans="1:7" ht="100" customHeight="1">
       <c r="A79" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
@@ -2750,30 +2655,28 @@
     </row>
     <row r="80" spans="1:7" ht="100" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="D80" s="7"/>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
     </row>
     <row r="81" spans="1:7" ht="100" customHeight="1">
       <c r="A81" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
@@ -2782,13 +2685,13 @@
     </row>
     <row r="82" spans="1:7" ht="100" customHeight="1">
       <c r="A82" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
@@ -2797,13 +2700,13 @@
     </row>
     <row r="83" spans="1:7" ht="100" customHeight="1">
       <c r="A83" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
@@ -2812,115 +2715,103 @@
     </row>
     <row r="84" spans="1:7" ht="100" customHeight="1">
       <c r="A84" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D84" s="7"/>
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
     </row>
     <row r="85" spans="1:7" ht="100" customHeight="1">
       <c r="A85" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="D85" s="7"/>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
     </row>
     <row r="86" spans="1:7" ht="100" customHeight="1">
       <c r="A86" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="D86" s="7"/>
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
     </row>
     <row r="87" spans="1:7" ht="100" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
     </row>
     <row r="88" spans="1:7" ht="100" customHeight="1">
       <c r="A88" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="D88" s="7"/>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
     </row>
     <row r="89" spans="1:7" ht="100" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="D89" s="7"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
     </row>
     <row r="90" spans="1:7" ht="100" customHeight="1">
       <c r="A90" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
@@ -2929,13 +2820,13 @@
     </row>
     <row r="91" spans="1:7" ht="100" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
@@ -2944,13 +2835,13 @@
     </row>
     <row r="92" spans="1:7" ht="100" customHeight="1">
       <c r="A92" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
@@ -2960,7 +2851,7 @@
     <row r="93" spans="1:7" ht="100" customHeight="1"/>
     <row r="94" spans="1:7">
       <c r="A94" s="6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>10</v>
@@ -2983,34 +2874,30 @@
     </row>
     <row r="95" spans="1:7" ht="100" customHeight="1">
       <c r="A95" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="D95" s="7"/>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
     </row>
     <row r="96" spans="1:7" ht="100" customHeight="1">
       <c r="A96" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D96" s="7"/>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
@@ -3018,7 +2905,7 @@
     <row r="97" spans="1:7" ht="100" customHeight="1"/>
     <row r="98" spans="1:7">
       <c r="A98" s="6" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>10</v>
@@ -3041,47 +2928,43 @@
     </row>
     <row r="99" spans="1:7" ht="100" customHeight="1">
       <c r="A99" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="D99" s="7"/>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
     </row>
     <row r="100" spans="1:7" ht="100" customHeight="1">
       <c r="A100" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="D100" s="7"/>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
     <row r="101" spans="1:7" ht="100" customHeight="1">
       <c r="A101" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
@@ -3090,17 +2973,15 @@
     </row>
     <row r="102" spans="1:7" ht="100" customHeight="1">
       <c r="A102" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="D102" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="D102" s="7"/>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
@@ -3108,7 +2989,7 @@
     <row r="103" spans="1:7" ht="100" customHeight="1"/>
     <row r="104" spans="1:7">
       <c r="A104" s="6" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>10</v>
@@ -3131,132 +3012,118 @@
     </row>
     <row r="105" spans="1:7" ht="100" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="D105" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="D105" s="7"/>
       <c r="E105" s="7"/>
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
     </row>
     <row r="106" spans="1:7" ht="100" customHeight="1">
       <c r="A106" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="D106" s="7"/>
       <c r="E106" s="7"/>
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
     </row>
     <row r="107" spans="1:7" ht="100" customHeight="1">
       <c r="A107" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="D107" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="D107" s="7"/>
       <c r="E107" s="7"/>
       <c r="F107" s="7"/>
       <c r="G107" s="7"/>
     </row>
     <row r="108" spans="1:7" ht="100" customHeight="1">
       <c r="A108" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="D108" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="D108" s="7"/>
       <c r="E108" s="7"/>
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
     </row>
     <row r="109" spans="1:7" ht="100" customHeight="1">
       <c r="A109" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="D109" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="D109" s="7"/>
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
     </row>
     <row r="110" spans="1:7" ht="100" customHeight="1">
       <c r="A110" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="D110" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="D110" s="7"/>
       <c r="E110" s="7"/>
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
     </row>
     <row r="111" spans="1:7" ht="100" customHeight="1">
       <c r="A111" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="D111" s="7"/>
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
       <c r="G111" s="7"/>
     </row>
     <row r="112" spans="1:7" ht="100" customHeight="1">
       <c r="A112" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
@@ -3265,13 +3132,13 @@
     </row>
     <row r="113" spans="1:7" ht="100" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
@@ -3280,13 +3147,13 @@
     </row>
     <row r="114" spans="1:7" ht="100" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
@@ -3296,7 +3163,7 @@
     <row r="115" spans="1:7" ht="100" customHeight="1"/>
     <row r="116" spans="1:7">
       <c r="A116" s="6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>10</v>
@@ -3319,30 +3186,28 @@
     </row>
     <row r="117" spans="1:7" ht="100" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="D117" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="D117" s="7"/>
       <c r="E117" s="7"/>
       <c r="F117" s="7"/>
       <c r="G117" s="7"/>
     </row>
     <row r="118" spans="1:7" ht="100" customHeight="1">
       <c r="A118" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
@@ -3351,30 +3216,28 @@
     </row>
     <row r="119" spans="1:7" ht="100" customHeight="1">
       <c r="A119" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="D119" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="D119" s="7"/>
       <c r="E119" s="7"/>
       <c r="F119" s="7"/>
       <c r="G119" s="7"/>
     </row>
     <row r="120" spans="1:7" ht="100" customHeight="1">
       <c r="A120" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D120" s="7"/>
       <c r="E120" s="7"/>
@@ -3383,13 +3246,13 @@
     </row>
     <row r="121" spans="1:7" ht="100" customHeight="1">
       <c r="A121" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
@@ -3398,13 +3261,13 @@
     </row>
     <row r="122" spans="1:7" ht="100" customHeight="1">
       <c r="A122" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D122" s="7"/>
       <c r="E122" s="7"/>
@@ -3413,13 +3276,13 @@
     </row>
     <row r="123" spans="1:7" ht="100" customHeight="1">
       <c r="A123" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D123" s="7"/>
       <c r="E123" s="7"/>
@@ -3428,13 +3291,13 @@
     </row>
     <row r="124" spans="1:7" ht="100" customHeight="1">
       <c r="A124" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
@@ -3443,30 +3306,28 @@
     </row>
     <row r="125" spans="1:7" ht="100" customHeight="1">
       <c r="A125" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="D125" s="7" t="s">
-        <v>19</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="D125" s="7"/>
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
     </row>
     <row r="126" spans="1:7" ht="100" customHeight="1">
       <c r="A126" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
@@ -3475,13 +3336,13 @@
     </row>
     <row r="127" spans="1:7" ht="100" customHeight="1">
       <c r="A127" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D127" s="7"/>
       <c r="E127" s="7"/>
@@ -3490,13 +3351,13 @@
     </row>
     <row r="128" spans="1:7" ht="100" customHeight="1">
       <c r="A128" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D128" s="7"/>
       <c r="E128" s="7"/>
@@ -3505,13 +3366,13 @@
     </row>
     <row r="129" spans="1:7" ht="100" customHeight="1">
       <c r="A129" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D129" s="7"/>
       <c r="E129" s="7"/>
@@ -3520,13 +3381,13 @@
     </row>
     <row r="130" spans="1:7" ht="100" customHeight="1">
       <c r="A130" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C130" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D130" s="7"/>
       <c r="E130" s="7"/>
@@ -3536,7 +3397,7 @@
     <row r="131" spans="1:7" ht="100" customHeight="1"/>
     <row r="132" spans="1:7">
       <c r="A132" s="6" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>10</v>
@@ -3559,13 +3420,13 @@
     </row>
     <row r="133" spans="1:7" ht="100" customHeight="1">
       <c r="A133" s="4" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>

</xml_diff>